<commit_message>
Fix randomness level to 3
</commit_message>
<xml_diff>
--- a/watch_list.xlsx
+++ b/watch_list.xlsx
@@ -444,7 +444,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H43"/>
+  <dimension ref="A1:H115"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -452,13 +452,13 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="10" customWidth="1" min="1" max="1"/>
+    <col width="11" customWidth="1" min="1" max="1"/>
     <col width="7" customWidth="1" min="2" max="2"/>
-    <col width="14" customWidth="1" min="3" max="3"/>
-    <col width="16" customWidth="1" min="4" max="4"/>
+    <col width="17" customWidth="1" min="3" max="3"/>
+    <col width="18" customWidth="1" min="4" max="4"/>
     <col width="17" customWidth="1" min="5" max="5"/>
     <col width="16" customWidth="1" min="6" max="6"/>
-    <col width="12" customWidth="1" min="7" max="7"/>
+    <col width="16" customWidth="1" min="7" max="7"/>
     <col width="6" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
@@ -1367,10 +1367,1507 @@
       <c r="G43" s="3" t="n"/>
       <c r="H43" s="3" t="n"/>
     </row>
+    <row r="44">
+      <c r="A44" s="3" t="n"/>
+      <c r="B44" s="3" t="inlineStr">
+        <is>
+          <t>20:00</t>
+        </is>
+      </c>
+      <c r="C44" s="3" t="inlineStr">
+        <is>
+          <t>אסרף
+לישי</t>
+        </is>
+      </c>
+      <c r="D44" s="3" t="inlineStr">
+        <is>
+          <t>לומיאנסקי
+ניסנוב</t>
+        </is>
+      </c>
+      <c r="E44" s="3" t="inlineStr">
+        <is>
+          <t>אור
+משה החופל</t>
+        </is>
+      </c>
+      <c r="F44" s="3" t="inlineStr">
+        <is>
+          <t>נפמן
+סדון</t>
+        </is>
+      </c>
+      <c r="G44" s="3" t="n"/>
+      <c r="H44" s="3" t="n"/>
+    </row>
+    <row r="45">
+      <c r="A45" s="3" t="n"/>
+      <c r="B45" s="3" t="inlineStr">
+        <is>
+          <t>21:00</t>
+        </is>
+      </c>
+      <c r="C45" s="3" t="n"/>
+      <c r="D45" s="3" t="n"/>
+      <c r="E45" s="3" t="n"/>
+      <c r="F45" s="3" t="n"/>
+      <c r="G45" s="3" t="n"/>
+      <c r="H45" s="3" t="n"/>
+    </row>
+    <row r="46">
+      <c r="A46" s="3" t="n"/>
+      <c r="B46" s="3" t="inlineStr">
+        <is>
+          <t>22:00</t>
+        </is>
+      </c>
+      <c r="C46" s="3" t="n"/>
+      <c r="D46" s="3" t="n"/>
+      <c r="E46" s="3" t="n"/>
+      <c r="F46" s="3" t="n"/>
+      <c r="G46" s="3" t="inlineStr">
+        <is>
+          <t>דותן
+שגיא</t>
+        </is>
+      </c>
+      <c r="H46" s="3" t="n"/>
+    </row>
+    <row r="47">
+      <c r="A47" s="3" t="n"/>
+      <c r="B47" s="3" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+      <c r="C47" s="3" t="inlineStr">
+        <is>
+          <t>דובר
+ליאור</t>
+        </is>
+      </c>
+      <c r="D47" s="3" t="inlineStr">
+        <is>
+          <t>אבנר
+רווה</t>
+        </is>
+      </c>
+      <c r="E47" s="3" t="inlineStr">
+        <is>
+          <t>כלפה
+קריספין</t>
+        </is>
+      </c>
+      <c r="F47" s="3" t="inlineStr">
+        <is>
+          <t>אסף
+משה</t>
+        </is>
+      </c>
+      <c r="G47" s="3" t="n"/>
+      <c r="H47" s="3" t="n"/>
+    </row>
+    <row r="48">
+      <c r="A48" s="3" t="inlineStr">
+        <is>
+          <t>Monday</t>
+        </is>
+      </c>
+      <c r="B48" s="3" t="inlineStr">
+        <is>
+          <t>00:00</t>
+        </is>
+      </c>
+      <c r="C48" s="3" t="n"/>
+      <c r="D48" s="3" t="n"/>
+      <c r="E48" s="3" t="n"/>
+      <c r="F48" s="3" t="n"/>
+      <c r="G48" s="3" t="n"/>
+      <c r="H48" s="3" t="n"/>
+    </row>
+    <row r="49">
+      <c r="A49" s="3" t="n"/>
+      <c r="B49" s="3" t="inlineStr">
+        <is>
+          <t>01:00</t>
+        </is>
+      </c>
+      <c r="C49" s="3" t="n"/>
+      <c r="D49" s="3" t="n"/>
+      <c r="E49" s="3" t="n"/>
+      <c r="F49" s="3" t="n"/>
+      <c r="G49" s="3" t="n"/>
+      <c r="H49" s="3" t="n"/>
+    </row>
+    <row r="50">
+      <c r="A50" s="3" t="n"/>
+      <c r="B50" s="3" t="inlineStr">
+        <is>
+          <t>02:00</t>
+        </is>
+      </c>
+      <c r="C50" s="3" t="inlineStr">
+        <is>
+          <t>אנזו
+שמעון</t>
+        </is>
+      </c>
+      <c r="D50" s="3" t="inlineStr">
+        <is>
+          <t>אנדי
+דוד</t>
+        </is>
+      </c>
+      <c r="E50" s="3" t="inlineStr">
+        <is>
+          <t>דימנטמן
+מטמוני</t>
+        </is>
+      </c>
+      <c r="F50" s="3" t="inlineStr">
+        <is>
+          <t>ארד
+יונג</t>
+        </is>
+      </c>
+      <c r="G50" s="3" t="inlineStr">
+        <is>
+          <t>לואיס
+לוטם</t>
+        </is>
+      </c>
+      <c r="H50" s="3" t="n"/>
+    </row>
+    <row r="51">
+      <c r="A51" s="3" t="n"/>
+      <c r="B51" s="3" t="inlineStr">
+        <is>
+          <t>03:00</t>
+        </is>
+      </c>
+      <c r="C51" s="3" t="n"/>
+      <c r="D51" s="3" t="n"/>
+      <c r="E51" s="3" t="n"/>
+      <c r="F51" s="3" t="n"/>
+      <c r="G51" s="3" t="n"/>
+      <c r="H51" s="3" t="n"/>
+    </row>
+    <row r="52">
+      <c r="A52" s="3" t="n"/>
+      <c r="B52" s="3" t="inlineStr">
+        <is>
+          <t>04:00</t>
+        </is>
+      </c>
+      <c r="C52" s="3" t="n"/>
+      <c r="D52" s="3" t="n"/>
+      <c r="E52" s="3" t="n"/>
+      <c r="F52" s="3" t="n"/>
+      <c r="G52" s="3" t="n"/>
+      <c r="H52" s="3" t="n"/>
+    </row>
+    <row r="53">
+      <c r="A53" s="3" t="n"/>
+      <c r="B53" s="3" t="inlineStr">
+        <is>
+          <t>05:00</t>
+        </is>
+      </c>
+      <c r="C53" s="3" t="inlineStr">
+        <is>
+          <t>איתי כהן
+אלכסיי</t>
+        </is>
+      </c>
+      <c r="D53" s="3" t="inlineStr">
+        <is>
+          <t>שראל
+שרעבי</t>
+        </is>
+      </c>
+      <c r="E53" s="3" t="inlineStr">
+        <is>
+          <t>אגומס
+פיאצה</t>
+        </is>
+      </c>
+      <c r="F53" s="3" t="inlineStr">
+        <is>
+          <t>דבוש
+דורון</t>
+        </is>
+      </c>
+      <c r="G53" s="3" t="n"/>
+      <c r="H53" s="3" t="n"/>
+    </row>
+    <row r="54">
+      <c r="A54" s="3" t="n"/>
+      <c r="B54" s="3" t="inlineStr">
+        <is>
+          <t>06:00</t>
+        </is>
+      </c>
+      <c r="C54" s="3" t="n"/>
+      <c r="D54" s="3" t="n"/>
+      <c r="E54" s="3" t="n"/>
+      <c r="F54" s="3" t="n"/>
+      <c r="G54" s="3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="H54" s="3" t="n"/>
+    </row>
+    <row r="55">
+      <c r="A55" s="3" t="n"/>
+      <c r="B55" s="3" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="C55" s="3" t="n"/>
+      <c r="D55" s="3" t="n"/>
+      <c r="E55" s="3" t="n"/>
+      <c r="F55" s="3" t="n"/>
+      <c r="G55" s="3" t="n"/>
+      <c r="H55" s="3" t="n"/>
+    </row>
+    <row r="56">
+      <c r="A56" s="3" t="n"/>
+      <c r="B56" s="3" t="inlineStr">
+        <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="C56" s="3" t="inlineStr">
+        <is>
+          <t>יואל
+סיני</t>
+        </is>
+      </c>
+      <c r="D56" s="3" t="inlineStr">
+        <is>
+          <t>דמיטרי
+עמיחי</t>
+        </is>
+      </c>
+      <c r="E56" s="3" t="inlineStr">
+        <is>
+          <t>דעאל
+שבצוב</t>
+        </is>
+      </c>
+      <c r="F56" s="3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G56" s="3" t="n"/>
+      <c r="H56" s="3" t="n"/>
+    </row>
+    <row r="57">
+      <c r="A57" s="3" t="n"/>
+      <c r="B57" s="3" t="inlineStr">
+        <is>
+          <t>09:00</t>
+        </is>
+      </c>
+      <c r="C57" s="3" t="n"/>
+      <c r="D57" s="3" t="n"/>
+      <c r="E57" s="3" t="n"/>
+      <c r="F57" s="3" t="n"/>
+      <c r="G57" s="3" t="n"/>
+      <c r="H57" s="3" t="n"/>
+    </row>
+    <row r="58">
+      <c r="A58" s="3" t="n"/>
+      <c r="B58" s="3" t="inlineStr">
+        <is>
+          <t>10:00</t>
+        </is>
+      </c>
+      <c r="C58" s="3" t="n"/>
+      <c r="D58" s="3" t="n"/>
+      <c r="E58" s="3" t="n"/>
+      <c r="F58" s="3" t="n"/>
+      <c r="G58" s="3" t="n"/>
+      <c r="H58" s="3" t="n"/>
+    </row>
+    <row r="59">
+      <c r="A59" s="3" t="n"/>
+      <c r="B59" s="3" t="inlineStr">
+        <is>
+          <t>11:00</t>
+        </is>
+      </c>
+      <c r="C59" s="3" t="inlineStr">
+        <is>
+          <t>אור
+אסרף</t>
+        </is>
+      </c>
+      <c r="D59" s="3" t="inlineStr">
+        <is>
+          <t>לומיאנסקי
+רוני</t>
+        </is>
+      </c>
+      <c r="E59" s="3" t="inlineStr">
+        <is>
+          <t>משה החופל
+נפמן</t>
+        </is>
+      </c>
+      <c r="F59" s="3" t="n"/>
+      <c r="G59" s="3" t="n"/>
+      <c r="H59" s="3" t="n"/>
+    </row>
+    <row r="60">
+      <c r="A60" s="3" t="n"/>
+      <c r="B60" s="3" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="C60" s="3" t="n"/>
+      <c r="D60" s="3" t="n"/>
+      <c r="E60" s="3" t="n"/>
+      <c r="F60" s="3" t="n"/>
+      <c r="G60" s="3" t="n"/>
+      <c r="H60" s="3" t="n"/>
+    </row>
+    <row r="61">
+      <c r="A61" s="3" t="n"/>
+      <c r="B61" s="3" t="inlineStr">
+        <is>
+          <t>13:00</t>
+        </is>
+      </c>
+      <c r="C61" s="3" t="n"/>
+      <c r="D61" s="3" t="n"/>
+      <c r="E61" s="3" t="n"/>
+      <c r="F61" s="3" t="n"/>
+      <c r="G61" s="3" t="n"/>
+      <c r="H61" s="3" t="n"/>
+    </row>
+    <row r="62">
+      <c r="A62" s="3" t="n"/>
+      <c r="B62" s="3" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="C62" s="3" t="inlineStr">
+        <is>
+          <t>לישי
+שגיא</t>
+        </is>
+      </c>
+      <c r="D62" s="3" t="inlineStr">
+        <is>
+          <t>ניסנוב
+סדון</t>
+        </is>
+      </c>
+      <c r="E62" s="3" t="inlineStr">
+        <is>
+          <t>דובר
+ליאור</t>
+        </is>
+      </c>
+      <c r="F62" s="3" t="n"/>
+      <c r="G62" s="3" t="n"/>
+      <c r="H62" s="3" t="n"/>
+    </row>
+    <row r="63">
+      <c r="A63" s="3" t="n"/>
+      <c r="B63" s="3" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="C63" s="3" t="n"/>
+      <c r="D63" s="3" t="n"/>
+      <c r="E63" s="3" t="n"/>
+      <c r="F63" s="3" t="n"/>
+      <c r="G63" s="3" t="n"/>
+      <c r="H63" s="3" t="n"/>
+    </row>
+    <row r="64">
+      <c r="A64" s="3" t="n"/>
+      <c r="B64" s="3" t="inlineStr">
+        <is>
+          <t>16:00</t>
+        </is>
+      </c>
+      <c r="C64" s="3" t="n"/>
+      <c r="D64" s="3" t="n"/>
+      <c r="E64" s="3" t="n"/>
+      <c r="F64" s="3" t="n"/>
+      <c r="G64" s="3" t="n"/>
+      <c r="H64" s="3" t="n"/>
+    </row>
+    <row r="65">
+      <c r="A65" s="3" t="n"/>
+      <c r="B65" s="3" t="inlineStr">
+        <is>
+          <t>17:00</t>
+        </is>
+      </c>
+      <c r="C65" s="3" t="inlineStr">
+        <is>
+          <t>כלפה
+רווה</t>
+        </is>
+      </c>
+      <c r="D65" s="3" t="inlineStr">
+        <is>
+          <t>אבנר
+קריספין</t>
+        </is>
+      </c>
+      <c r="E65" s="3" t="inlineStr">
+        <is>
+          <t>דותן
+משה</t>
+        </is>
+      </c>
+      <c r="F65" s="3" t="n"/>
+      <c r="G65" s="3" t="n"/>
+      <c r="H65" s="3" t="n"/>
+    </row>
+    <row r="66">
+      <c r="A66" s="3" t="n"/>
+      <c r="B66" s="3" t="inlineStr">
+        <is>
+          <t>18:00</t>
+        </is>
+      </c>
+      <c r="C66" s="3" t="n"/>
+      <c r="D66" s="3" t="n"/>
+      <c r="E66" s="3" t="n"/>
+      <c r="F66" s="3" t="n"/>
+      <c r="G66" s="3" t="n"/>
+      <c r="H66" s="3" t="n"/>
+    </row>
+    <row r="67">
+      <c r="A67" s="3" t="n"/>
+      <c r="B67" s="3" t="inlineStr">
+        <is>
+          <t>19:00</t>
+        </is>
+      </c>
+      <c r="C67" s="3" t="n"/>
+      <c r="D67" s="3" t="n"/>
+      <c r="E67" s="3" t="n"/>
+      <c r="F67" s="3" t="n"/>
+      <c r="G67" s="3" t="n"/>
+      <c r="H67" s="3" t="n"/>
+    </row>
+    <row r="68">
+      <c r="A68" s="3" t="n"/>
+      <c r="B68" s="3" t="inlineStr">
+        <is>
+          <t>20:00</t>
+        </is>
+      </c>
+      <c r="C68" s="3" t="inlineStr">
+        <is>
+          <t>אנדי
+דוד</t>
+        </is>
+      </c>
+      <c r="D68" s="3" t="inlineStr">
+        <is>
+          <t>אנזו
+ארד</t>
+        </is>
+      </c>
+      <c r="E68" s="3" t="inlineStr">
+        <is>
+          <t>אסף
+שמעון</t>
+        </is>
+      </c>
+      <c r="F68" s="3" t="inlineStr">
+        <is>
+          <t>יונג
+לואיס</t>
+        </is>
+      </c>
+      <c r="G68" s="3" t="n"/>
+      <c r="H68" s="3" t="n"/>
+    </row>
+    <row r="69">
+      <c r="A69" s="3" t="n"/>
+      <c r="B69" s="3" t="inlineStr">
+        <is>
+          <t>21:00</t>
+        </is>
+      </c>
+      <c r="C69" s="3" t="n"/>
+      <c r="D69" s="3" t="n"/>
+      <c r="E69" s="3" t="n"/>
+      <c r="F69" s="3" t="n"/>
+      <c r="G69" s="3" t="n"/>
+      <c r="H69" s="3" t="n"/>
+    </row>
+    <row r="70">
+      <c r="A70" s="3" t="n"/>
+      <c r="B70" s="3" t="inlineStr">
+        <is>
+          <t>22:00</t>
+        </is>
+      </c>
+      <c r="C70" s="3" t="n"/>
+      <c r="D70" s="3" t="n"/>
+      <c r="E70" s="3" t="n"/>
+      <c r="F70" s="3" t="n"/>
+      <c r="G70" s="3" t="inlineStr">
+        <is>
+          <t>דימנטמן
+מטמוני</t>
+        </is>
+      </c>
+      <c r="H70" s="3" t="n"/>
+    </row>
+    <row r="71">
+      <c r="A71" s="3" t="n"/>
+      <c r="B71" s="3" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+      <c r="C71" s="3" t="inlineStr">
+        <is>
+          <t>אלכסיי
+לוטם</t>
+        </is>
+      </c>
+      <c r="D71" s="3" t="inlineStr">
+        <is>
+          <t>דורון
+שראל</t>
+        </is>
+      </c>
+      <c r="E71" s="3" t="inlineStr">
+        <is>
+          <t>דבוש
+פיאצה</t>
+        </is>
+      </c>
+      <c r="F71" s="3" t="inlineStr">
+        <is>
+          <t>אגומס
+איתי כהן</t>
+        </is>
+      </c>
+      <c r="G71" s="3" t="n"/>
+      <c r="H71" s="3" t="n"/>
+    </row>
+    <row r="72">
+      <c r="A72" s="3" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="B72" s="3" t="inlineStr">
+        <is>
+          <t>00:00</t>
+        </is>
+      </c>
+      <c r="C72" s="3" t="n"/>
+      <c r="D72" s="3" t="n"/>
+      <c r="E72" s="3" t="n"/>
+      <c r="F72" s="3" t="n"/>
+      <c r="G72" s="3" t="n"/>
+      <c r="H72" s="3" t="n"/>
+    </row>
+    <row r="73">
+      <c r="A73" s="3" t="n"/>
+      <c r="B73" s="3" t="inlineStr">
+        <is>
+          <t>01:00</t>
+        </is>
+      </c>
+      <c r="C73" s="3" t="n"/>
+      <c r="D73" s="3" t="n"/>
+      <c r="E73" s="3" t="n"/>
+      <c r="F73" s="3" t="n"/>
+      <c r="G73" s="3" t="n"/>
+      <c r="H73" s="3" t="n"/>
+    </row>
+    <row r="74">
+      <c r="A74" s="3" t="n"/>
+      <c r="B74" s="3" t="inlineStr">
+        <is>
+          <t>02:00</t>
+        </is>
+      </c>
+      <c r="C74" s="3" t="inlineStr">
+        <is>
+          <t>סיני
+שרעבי</t>
+        </is>
+      </c>
+      <c r="D74" s="3" t="inlineStr">
+        <is>
+          <t>דעאל
+יואל</t>
+        </is>
+      </c>
+      <c r="E74" s="3" t="inlineStr">
+        <is>
+          <t>דמיטרי
+עמיחי</t>
+        </is>
+      </c>
+      <c r="F74" s="3" t="inlineStr">
+        <is>
+          <t>רוני
+שבצוב</t>
+        </is>
+      </c>
+      <c r="G74" s="3" t="inlineStr">
+        <is>
+          <t>אסרף
+לישי</t>
+        </is>
+      </c>
+      <c r="H74" s="3" t="n"/>
+    </row>
+    <row r="75">
+      <c r="A75" s="3" t="n"/>
+      <c r="B75" s="3" t="inlineStr">
+        <is>
+          <t>03:00</t>
+        </is>
+      </c>
+      <c r="C75" s="3" t="n"/>
+      <c r="D75" s="3" t="n"/>
+      <c r="E75" s="3" t="n"/>
+      <c r="F75" s="3" t="n"/>
+      <c r="G75" s="3" t="n"/>
+      <c r="H75" s="3" t="n"/>
+    </row>
+    <row r="76">
+      <c r="A76" s="3" t="n"/>
+      <c r="B76" s="3" t="inlineStr">
+        <is>
+          <t>04:00</t>
+        </is>
+      </c>
+      <c r="C76" s="3" t="n"/>
+      <c r="D76" s="3" t="n"/>
+      <c r="E76" s="3" t="n"/>
+      <c r="F76" s="3" t="n"/>
+      <c r="G76" s="3" t="n"/>
+      <c r="H76" s="3" t="n"/>
+    </row>
+    <row r="77">
+      <c r="A77" s="3" t="n"/>
+      <c r="B77" s="3" t="inlineStr">
+        <is>
+          <t>05:00</t>
+        </is>
+      </c>
+      <c r="C77" s="3" t="inlineStr">
+        <is>
+          <t>אור
+משה החופל</t>
+        </is>
+      </c>
+      <c r="D77" s="3" t="inlineStr">
+        <is>
+          <t>לומיאנסקי
+סדון</t>
+        </is>
+      </c>
+      <c r="E77" s="3" t="inlineStr">
+        <is>
+          <t>דותן
+שגיא</t>
+        </is>
+      </c>
+      <c r="F77" s="3" t="inlineStr">
+        <is>
+          <t>אבנר
+נפמן</t>
+        </is>
+      </c>
+      <c r="G77" s="3" t="n"/>
+      <c r="H77" s="3" t="n"/>
+    </row>
+    <row r="78">
+      <c r="A78" s="3" t="n"/>
+      <c r="B78" s="3" t="inlineStr">
+        <is>
+          <t>06:00</t>
+        </is>
+      </c>
+      <c r="C78" s="3" t="n"/>
+      <c r="D78" s="3" t="n"/>
+      <c r="E78" s="3" t="n"/>
+      <c r="F78" s="3" t="n"/>
+      <c r="G78" s="3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="H78" s="3" t="n"/>
+    </row>
+    <row r="79">
+      <c r="A79" s="3" t="n"/>
+      <c r="B79" s="3" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="C79" s="3" t="n"/>
+      <c r="D79" s="3" t="n"/>
+      <c r="E79" s="3" t="n"/>
+      <c r="F79" s="3" t="n"/>
+      <c r="G79" s="3" t="n"/>
+      <c r="H79" s="3" t="n"/>
+    </row>
+    <row r="80">
+      <c r="A80" s="3" t="n"/>
+      <c r="B80" s="3" t="inlineStr">
+        <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="C80" s="3" t="inlineStr">
+        <is>
+          <t>דובר
+ניסנוב</t>
+        </is>
+      </c>
+      <c r="D80" s="3" t="inlineStr">
+        <is>
+          <t>כלפה
+קריספין</t>
+        </is>
+      </c>
+      <c r="E80" s="3" t="inlineStr">
+        <is>
+          <t>ליאור
+רווה</t>
+        </is>
+      </c>
+      <c r="F80" s="3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G80" s="3" t="n"/>
+      <c r="H80" s="3" t="n"/>
+    </row>
+    <row r="81">
+      <c r="A81" s="3" t="n"/>
+      <c r="B81" s="3" t="inlineStr">
+        <is>
+          <t>09:00</t>
+        </is>
+      </c>
+      <c r="C81" s="3" t="n"/>
+      <c r="D81" s="3" t="n"/>
+      <c r="E81" s="3" t="n"/>
+      <c r="F81" s="3" t="n"/>
+      <c r="G81" s="3" t="n"/>
+      <c r="H81" s="3" t="n"/>
+    </row>
+    <row r="82">
+      <c r="A82" s="3" t="n"/>
+      <c r="B82" s="3" t="inlineStr">
+        <is>
+          <t>10:00</t>
+        </is>
+      </c>
+      <c r="C82" s="3" t="n"/>
+      <c r="D82" s="3" t="n"/>
+      <c r="E82" s="3" t="n"/>
+      <c r="F82" s="3" t="n"/>
+      <c r="G82" s="3" t="n"/>
+      <c r="H82" s="3" t="n"/>
+    </row>
+    <row r="83">
+      <c r="A83" s="3" t="n"/>
+      <c r="B83" s="3" t="inlineStr">
+        <is>
+          <t>11:00</t>
+        </is>
+      </c>
+      <c r="C83" s="3" t="inlineStr">
+        <is>
+          <t>אסף
+ארד</t>
+        </is>
+      </c>
+      <c r="D83" s="3" t="inlineStr">
+        <is>
+          <t>אנדי
+דוד</t>
+        </is>
+      </c>
+      <c r="E83" s="3" t="inlineStr">
+        <is>
+          <t>אנזו
+משה</t>
+        </is>
+      </c>
+      <c r="F83" s="3" t="n"/>
+      <c r="G83" s="3" t="n"/>
+      <c r="H83" s="3" t="n"/>
+    </row>
+    <row r="84">
+      <c r="A84" s="3" t="n"/>
+      <c r="B84" s="3" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="C84" s="3" t="n"/>
+      <c r="D84" s="3" t="n"/>
+      <c r="E84" s="3" t="n"/>
+      <c r="F84" s="3" t="n"/>
+      <c r="G84" s="3" t="n"/>
+      <c r="H84" s="3" t="n"/>
+    </row>
+    <row r="85">
+      <c r="A85" s="3" t="n"/>
+      <c r="B85" s="3" t="inlineStr">
+        <is>
+          <t>13:00</t>
+        </is>
+      </c>
+      <c r="C85" s="3" t="n"/>
+      <c r="D85" s="3" t="n"/>
+      <c r="E85" s="3" t="n"/>
+      <c r="F85" s="3" t="n"/>
+      <c r="G85" s="3" t="n"/>
+      <c r="H85" s="3" t="n"/>
+    </row>
+    <row r="86">
+      <c r="A86" s="3" t="n"/>
+      <c r="B86" s="3" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="C86" s="3" t="inlineStr">
+        <is>
+          <t>יונג
+שמעון</t>
+        </is>
+      </c>
+      <c r="D86" s="3" t="inlineStr">
+        <is>
+          <t>דימנטמן
+מטמוני</t>
+        </is>
+      </c>
+      <c r="E86" s="3" t="inlineStr">
+        <is>
+          <t>אלכסיי
+לואיס</t>
+        </is>
+      </c>
+      <c r="F86" s="3" t="n"/>
+      <c r="G86" s="3" t="n"/>
+      <c r="H86" s="3" t="n"/>
+    </row>
+    <row r="87">
+      <c r="A87" s="3" t="n"/>
+      <c r="B87" s="3" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="C87" s="3" t="n"/>
+      <c r="D87" s="3" t="n"/>
+      <c r="E87" s="3" t="n"/>
+      <c r="F87" s="3" t="n"/>
+      <c r="G87" s="3" t="n"/>
+      <c r="H87" s="3" t="n"/>
+    </row>
+    <row r="88">
+      <c r="A88" s="3" t="n"/>
+      <c r="B88" s="3" t="inlineStr">
+        <is>
+          <t>16:00</t>
+        </is>
+      </c>
+      <c r="C88" s="3" t="n"/>
+      <c r="D88" s="3" t="n"/>
+      <c r="E88" s="3" t="n"/>
+      <c r="F88" s="3" t="n"/>
+      <c r="G88" s="3" t="n"/>
+      <c r="H88" s="3" t="n"/>
+    </row>
+    <row r="89">
+      <c r="A89" s="3" t="n"/>
+      <c r="B89" s="3" t="inlineStr">
+        <is>
+          <t>17:00</t>
+        </is>
+      </c>
+      <c r="C89" s="3" t="inlineStr">
+        <is>
+          <t>איתי כהן
+דורון</t>
+        </is>
+      </c>
+      <c r="D89" s="3" t="inlineStr">
+        <is>
+          <t>דבוש
+לוטם</t>
+        </is>
+      </c>
+      <c r="E89" s="3" t="inlineStr">
+        <is>
+          <t>שראל
+שרעבי</t>
+        </is>
+      </c>
+      <c r="F89" s="3" t="n"/>
+      <c r="G89" s="3" t="n"/>
+      <c r="H89" s="3" t="n"/>
+    </row>
+    <row r="90">
+      <c r="A90" s="3" t="n"/>
+      <c r="B90" s="3" t="inlineStr">
+        <is>
+          <t>18:00</t>
+        </is>
+      </c>
+      <c r="C90" s="3" t="n"/>
+      <c r="D90" s="3" t="n"/>
+      <c r="E90" s="3" t="n"/>
+      <c r="F90" s="3" t="n"/>
+      <c r="G90" s="3" t="n"/>
+      <c r="H90" s="3" t="n"/>
+    </row>
+    <row r="91">
+      <c r="A91" s="3" t="n"/>
+      <c r="B91" s="3" t="inlineStr">
+        <is>
+          <t>19:00</t>
+        </is>
+      </c>
+      <c r="C91" s="3" t="n"/>
+      <c r="D91" s="3" t="n"/>
+      <c r="E91" s="3" t="n"/>
+      <c r="F91" s="3" t="n"/>
+      <c r="G91" s="3" t="n"/>
+      <c r="H91" s="3" t="n"/>
+    </row>
+    <row r="92">
+      <c r="A92" s="3" t="n"/>
+      <c r="B92" s="3" t="inlineStr">
+        <is>
+          <t>20:00</t>
+        </is>
+      </c>
+      <c r="C92" s="3" t="inlineStr">
+        <is>
+          <t>אגומס
+סיני</t>
+        </is>
+      </c>
+      <c r="D92" s="3" t="inlineStr">
+        <is>
+          <t>דעאל
+עמיחי</t>
+        </is>
+      </c>
+      <c r="E92" s="3" t="inlineStr">
+        <is>
+          <t>יואל
+רוני</t>
+        </is>
+      </c>
+      <c r="F92" s="3" t="inlineStr">
+        <is>
+          <t>דמיטרי
+שבצוב</t>
+        </is>
+      </c>
+      <c r="G92" s="3" t="n"/>
+      <c r="H92" s="3" t="n"/>
+    </row>
+    <row r="93">
+      <c r="A93" s="3" t="n"/>
+      <c r="B93" s="3" t="inlineStr">
+        <is>
+          <t>21:00</t>
+        </is>
+      </c>
+      <c r="C93" s="3" t="n"/>
+      <c r="D93" s="3" t="n"/>
+      <c r="E93" s="3" t="n"/>
+      <c r="F93" s="3" t="n"/>
+      <c r="G93" s="3" t="n"/>
+      <c r="H93" s="3" t="n"/>
+    </row>
+    <row r="94">
+      <c r="A94" s="3" t="n"/>
+      <c r="B94" s="3" t="inlineStr">
+        <is>
+          <t>22:00</t>
+        </is>
+      </c>
+      <c r="C94" s="3" t="n"/>
+      <c r="D94" s="3" t="n"/>
+      <c r="E94" s="3" t="n"/>
+      <c r="F94" s="3" t="n"/>
+      <c r="G94" s="3" t="inlineStr">
+        <is>
+          <t>אור
+אסרף</t>
+        </is>
+      </c>
+      <c r="H94" s="3" t="n"/>
+    </row>
+    <row r="95">
+      <c r="A95" s="3" t="n"/>
+      <c r="B95" s="3" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+      <c r="C95" s="3" t="inlineStr">
+        <is>
+          <t>לישי
+פיאצה</t>
+        </is>
+      </c>
+      <c r="D95" s="3" t="inlineStr">
+        <is>
+          <t>ניסנוב
+נפמן</t>
+        </is>
+      </c>
+      <c r="E95" s="3" t="inlineStr">
+        <is>
+          <t>משה החופל
+שגיא</t>
+        </is>
+      </c>
+      <c r="F95" s="3" t="inlineStr">
+        <is>
+          <t>דותן
+לומיאנסקי</t>
+        </is>
+      </c>
+      <c r="G95" s="3" t="n"/>
+      <c r="H95" s="3" t="n"/>
+    </row>
+    <row r="96">
+      <c r="A96" s="3" t="inlineStr">
+        <is>
+          <t>Wednesday</t>
+        </is>
+      </c>
+      <c r="B96" s="3" t="inlineStr">
+        <is>
+          <t>00:00</t>
+        </is>
+      </c>
+      <c r="C96" s="3" t="n"/>
+      <c r="D96" s="3" t="n"/>
+      <c r="E96" s="3" t="n"/>
+      <c r="F96" s="3" t="n"/>
+      <c r="G96" s="3" t="n"/>
+      <c r="H96" s="3" t="n"/>
+    </row>
+    <row r="97">
+      <c r="A97" s="3" t="n"/>
+      <c r="B97" s="3" t="inlineStr">
+        <is>
+          <t>01:00</t>
+        </is>
+      </c>
+      <c r="C97" s="3" t="n"/>
+      <c r="D97" s="3" t="n"/>
+      <c r="E97" s="3" t="n"/>
+      <c r="F97" s="3" t="n"/>
+      <c r="G97" s="3" t="n"/>
+      <c r="H97" s="3" t="n"/>
+    </row>
+    <row r="98">
+      <c r="A98" s="3" t="n"/>
+      <c r="B98" s="3" t="inlineStr">
+        <is>
+          <t>02:00</t>
+        </is>
+      </c>
+      <c r="C98" s="3" t="inlineStr">
+        <is>
+          <t>אבנר
+דובר</t>
+        </is>
+      </c>
+      <c r="D98" s="3" t="inlineStr">
+        <is>
+          <t>כלפה
+סדון</t>
+        </is>
+      </c>
+      <c r="E98" s="3" t="inlineStr">
+        <is>
+          <t>ארד
+רווה</t>
+        </is>
+      </c>
+      <c r="F98" s="3" t="inlineStr">
+        <is>
+          <t>ליאור
+קריספין</t>
+        </is>
+      </c>
+      <c r="G98" s="3" t="inlineStr">
+        <is>
+          <t>אסף
+משה</t>
+        </is>
+      </c>
+      <c r="H98" s="3" t="n"/>
+    </row>
+    <row r="99">
+      <c r="A99" s="3" t="n"/>
+      <c r="B99" s="3" t="inlineStr">
+        <is>
+          <t>03:00</t>
+        </is>
+      </c>
+      <c r="C99" s="3" t="n"/>
+      <c r="D99" s="3" t="n"/>
+      <c r="E99" s="3" t="n"/>
+      <c r="F99" s="3" t="n"/>
+      <c r="G99" s="3" t="n"/>
+      <c r="H99" s="3" t="n"/>
+    </row>
+    <row r="100">
+      <c r="A100" s="3" t="n"/>
+      <c r="B100" s="3" t="inlineStr">
+        <is>
+          <t>04:00</t>
+        </is>
+      </c>
+      <c r="C100" s="3" t="n"/>
+      <c r="D100" s="3" t="n"/>
+      <c r="E100" s="3" t="n"/>
+      <c r="F100" s="3" t="n"/>
+      <c r="G100" s="3" t="n"/>
+      <c r="H100" s="3" t="n"/>
+    </row>
+    <row r="101">
+      <c r="A101" s="3" t="n"/>
+      <c r="B101" s="3" t="inlineStr">
+        <is>
+          <t>05:00</t>
+        </is>
+      </c>
+      <c r="C101" s="3" t="inlineStr">
+        <is>
+          <t>אנדי
+דוד</t>
+        </is>
+      </c>
+      <c r="D101" s="3" t="inlineStr">
+        <is>
+          <t>אנזו
+שמעון</t>
+        </is>
+      </c>
+      <c r="E101" s="3" t="inlineStr">
+        <is>
+          <t>דימנטמן
+מטמוני</t>
+        </is>
+      </c>
+      <c r="F101" s="3" t="inlineStr">
+        <is>
+          <t>אלכסיי
+דורון</t>
+        </is>
+      </c>
+      <c r="G101" s="3" t="n"/>
+      <c r="H101" s="3" t="n"/>
+    </row>
+    <row r="102">
+      <c r="A102" s="3" t="n"/>
+      <c r="B102" s="3" t="inlineStr">
+        <is>
+          <t>06:00</t>
+        </is>
+      </c>
+      <c r="C102" s="3" t="n"/>
+      <c r="D102" s="3" t="n"/>
+      <c r="E102" s="3" t="n"/>
+      <c r="F102" s="3" t="n"/>
+      <c r="G102" s="3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="H102" s="3" t="n"/>
+    </row>
+    <row r="103">
+      <c r="A103" s="3" t="n"/>
+      <c r="B103" s="3" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="C103" s="3" t="n"/>
+      <c r="D103" s="3" t="n"/>
+      <c r="E103" s="3" t="n"/>
+      <c r="F103" s="3" t="n"/>
+      <c r="G103" s="3" t="n"/>
+      <c r="H103" s="3" t="n"/>
+    </row>
+    <row r="104">
+      <c r="A104" s="3" t="n"/>
+      <c r="B104" s="3" t="inlineStr">
+        <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="C104" s="3" t="inlineStr">
+        <is>
+          <t>לואיס
+לוטם</t>
+        </is>
+      </c>
+      <c r="D104" s="3" t="inlineStr">
+        <is>
+          <t>איתי כהן
+שרעבי</t>
+        </is>
+      </c>
+      <c r="E104" s="3" t="inlineStr">
+        <is>
+          <t>דבוש
+שראל</t>
+        </is>
+      </c>
+      <c r="F104" s="3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G104" s="3" t="n"/>
+      <c r="H104" s="3" t="n"/>
+    </row>
+    <row r="105">
+      <c r="A105" s="3" t="n"/>
+      <c r="B105" s="3" t="inlineStr">
+        <is>
+          <t>09:00</t>
+        </is>
+      </c>
+      <c r="C105" s="3" t="n"/>
+      <c r="D105" s="3" t="n"/>
+      <c r="E105" s="3" t="n"/>
+      <c r="F105" s="3" t="n"/>
+      <c r="G105" s="3" t="n"/>
+      <c r="H105" s="3" t="n"/>
+    </row>
+    <row r="106">
+      <c r="A106" s="3" t="n"/>
+      <c r="B106" s="3" t="inlineStr">
+        <is>
+          <t>10:00</t>
+        </is>
+      </c>
+      <c r="C106" s="3" t="n"/>
+      <c r="D106" s="3" t="n"/>
+      <c r="E106" s="3" t="n"/>
+      <c r="F106" s="3" t="n"/>
+      <c r="G106" s="3" t="n"/>
+      <c r="H106" s="3" t="n"/>
+    </row>
+    <row r="107">
+      <c r="A107" s="3" t="n"/>
+      <c r="B107" s="3" t="inlineStr">
+        <is>
+          <t>11:00</t>
+        </is>
+      </c>
+      <c r="C107" s="3" t="inlineStr">
+        <is>
+          <t>אגומס
+פיאצה</t>
+        </is>
+      </c>
+      <c r="D107" s="3" t="inlineStr">
+        <is>
+          <t>יונג
+עמיחי</t>
+        </is>
+      </c>
+      <c r="E107" s="3" t="inlineStr">
+        <is>
+          <t>יואל
+סיני</t>
+        </is>
+      </c>
+      <c r="F107" s="3" t="n"/>
+      <c r="G107" s="3" t="n"/>
+      <c r="H107" s="3" t="n"/>
+    </row>
+    <row r="108">
+      <c r="A108" s="3" t="n"/>
+      <c r="B108" s="3" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="C108" s="3" t="n"/>
+      <c r="D108" s="3" t="n"/>
+      <c r="E108" s="3" t="n"/>
+      <c r="F108" s="3" t="n"/>
+      <c r="G108" s="3" t="n"/>
+      <c r="H108" s="3" t="n"/>
+    </row>
+    <row r="109">
+      <c r="A109" s="3" t="n"/>
+      <c r="B109" s="3" t="inlineStr">
+        <is>
+          <t>13:00</t>
+        </is>
+      </c>
+      <c r="C109" s="3" t="n"/>
+      <c r="D109" s="3" t="n"/>
+      <c r="E109" s="3" t="n"/>
+      <c r="F109" s="3" t="n"/>
+      <c r="G109" s="3" t="n"/>
+      <c r="H109" s="3" t="n"/>
+    </row>
+    <row r="110">
+      <c r="A110" s="3" t="n"/>
+      <c r="B110" s="3" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="C110" s="3" t="inlineStr">
+        <is>
+          <t>דעאל
+רוני</t>
+        </is>
+      </c>
+      <c r="D110" s="3" t="inlineStr">
+        <is>
+          <t>דמיטרי
+לישי</t>
+        </is>
+      </c>
+      <c r="E110" s="3" t="inlineStr">
+        <is>
+          <t>אסרף
+שבצוב</t>
+        </is>
+      </c>
+      <c r="F110" s="3" t="n"/>
+      <c r="G110" s="3" t="n"/>
+      <c r="H110" s="3" t="n"/>
+    </row>
+    <row r="111">
+      <c r="A111" s="3" t="n"/>
+      <c r="B111" s="3" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="C111" s="3" t="n"/>
+      <c r="D111" s="3" t="n"/>
+      <c r="E111" s="3" t="n"/>
+      <c r="F111" s="3" t="n"/>
+      <c r="G111" s="3" t="n"/>
+      <c r="H111" s="3" t="n"/>
+    </row>
+    <row r="112">
+      <c r="A112" s="3" t="n"/>
+      <c r="B112" s="3" t="inlineStr">
+        <is>
+          <t>16:00</t>
+        </is>
+      </c>
+      <c r="C112" s="3" t="n"/>
+      <c r="D112" s="3" t="n"/>
+      <c r="E112" s="3" t="n"/>
+      <c r="F112" s="3" t="n"/>
+      <c r="G112" s="3" t="n"/>
+      <c r="H112" s="3" t="n"/>
+    </row>
+    <row r="113">
+      <c r="A113" s="3" t="n"/>
+      <c r="B113" s="3" t="inlineStr">
+        <is>
+          <t>17:00</t>
+        </is>
+      </c>
+      <c r="C113" s="3" t="inlineStr">
+        <is>
+          <t>אור
+ניסנוב</t>
+        </is>
+      </c>
+      <c r="D113" s="3" t="inlineStr">
+        <is>
+          <t>משה החופל
+נפמן</t>
+        </is>
+      </c>
+      <c r="E113" s="3" t="inlineStr">
+        <is>
+          <t>לומיאנסקי
+סדון</t>
+        </is>
+      </c>
+      <c r="F113" s="3" t="n"/>
+      <c r="G113" s="3" t="n"/>
+      <c r="H113" s="3" t="n"/>
+    </row>
+    <row r="114">
+      <c r="A114" s="3" t="n"/>
+      <c r="B114" s="3" t="inlineStr">
+        <is>
+          <t>18:00</t>
+        </is>
+      </c>
+      <c r="C114" s="3" t="n"/>
+      <c r="D114" s="3" t="n"/>
+      <c r="E114" s="3" t="n"/>
+      <c r="F114" s="3" t="n"/>
+      <c r="G114" s="3" t="n"/>
+      <c r="H114" s="3" t="n"/>
+    </row>
+    <row r="115">
+      <c r="A115" s="3" t="n"/>
+      <c r="B115" s="3" t="inlineStr">
+        <is>
+          <t>19:00</t>
+        </is>
+      </c>
+      <c r="C115" s="3" t="n"/>
+      <c r="D115" s="3" t="n"/>
+      <c r="E115" s="3" t="n"/>
+      <c r="F115" s="3" t="n"/>
+      <c r="G115" s="3" t="n"/>
+      <c r="H115" s="3" t="n"/>
+    </row>
   </sheetData>
-  <mergeCells count="57">
+  <mergeCells count="156">
     <mergeCell ref="A2:A23"/>
-    <mergeCell ref="A24:A43"/>
+    <mergeCell ref="A24:A47"/>
+    <mergeCell ref="A48:A71"/>
+    <mergeCell ref="A72:A95"/>
+    <mergeCell ref="A96:A115"/>
     <mergeCell ref="C2:C4"/>
     <mergeCell ref="C5:C7"/>
     <mergeCell ref="C8:C10"/>
@@ -1385,6 +2882,30 @@
     <mergeCell ref="C35:C37"/>
     <mergeCell ref="C38:C40"/>
     <mergeCell ref="C41:C43"/>
+    <mergeCell ref="C44:C46"/>
+    <mergeCell ref="C47:C49"/>
+    <mergeCell ref="C50:C52"/>
+    <mergeCell ref="C53:C55"/>
+    <mergeCell ref="C56:C58"/>
+    <mergeCell ref="C59:C61"/>
+    <mergeCell ref="C62:C64"/>
+    <mergeCell ref="C65:C67"/>
+    <mergeCell ref="C68:C70"/>
+    <mergeCell ref="C71:C73"/>
+    <mergeCell ref="C74:C76"/>
+    <mergeCell ref="C77:C79"/>
+    <mergeCell ref="C80:C82"/>
+    <mergeCell ref="C83:C85"/>
+    <mergeCell ref="C86:C88"/>
+    <mergeCell ref="C89:C91"/>
+    <mergeCell ref="C92:C94"/>
+    <mergeCell ref="C95:C97"/>
+    <mergeCell ref="C98:C100"/>
+    <mergeCell ref="C101:C103"/>
+    <mergeCell ref="C104:C106"/>
+    <mergeCell ref="C107:C109"/>
+    <mergeCell ref="C110:C112"/>
+    <mergeCell ref="C113:C115"/>
     <mergeCell ref="D2:D4"/>
     <mergeCell ref="D5:D7"/>
     <mergeCell ref="D8:D10"/>
@@ -1399,6 +2920,30 @@
     <mergeCell ref="D35:D37"/>
     <mergeCell ref="D38:D40"/>
     <mergeCell ref="D41:D43"/>
+    <mergeCell ref="D44:D46"/>
+    <mergeCell ref="D47:D49"/>
+    <mergeCell ref="D50:D52"/>
+    <mergeCell ref="D53:D55"/>
+    <mergeCell ref="D56:D58"/>
+    <mergeCell ref="D59:D61"/>
+    <mergeCell ref="D62:D64"/>
+    <mergeCell ref="D65:D67"/>
+    <mergeCell ref="D68:D70"/>
+    <mergeCell ref="D71:D73"/>
+    <mergeCell ref="D74:D76"/>
+    <mergeCell ref="D77:D79"/>
+    <mergeCell ref="D80:D82"/>
+    <mergeCell ref="D83:D85"/>
+    <mergeCell ref="D86:D88"/>
+    <mergeCell ref="D89:D91"/>
+    <mergeCell ref="D92:D94"/>
+    <mergeCell ref="D95:D97"/>
+    <mergeCell ref="D98:D100"/>
+    <mergeCell ref="D101:D103"/>
+    <mergeCell ref="D104:D106"/>
+    <mergeCell ref="D107:D109"/>
+    <mergeCell ref="D110:D112"/>
+    <mergeCell ref="D113:D115"/>
     <mergeCell ref="E2:E4"/>
     <mergeCell ref="E5:E7"/>
     <mergeCell ref="E8:E10"/>
@@ -1413,6 +2958,30 @@
     <mergeCell ref="E35:E37"/>
     <mergeCell ref="E38:E40"/>
     <mergeCell ref="E41:E43"/>
+    <mergeCell ref="E44:E46"/>
+    <mergeCell ref="E47:E49"/>
+    <mergeCell ref="E50:E52"/>
+    <mergeCell ref="E53:E55"/>
+    <mergeCell ref="E56:E58"/>
+    <mergeCell ref="E59:E61"/>
+    <mergeCell ref="E62:E64"/>
+    <mergeCell ref="E65:E67"/>
+    <mergeCell ref="E68:E70"/>
+    <mergeCell ref="E71:E73"/>
+    <mergeCell ref="E74:E76"/>
+    <mergeCell ref="E77:E79"/>
+    <mergeCell ref="E80:E82"/>
+    <mergeCell ref="E83:E85"/>
+    <mergeCell ref="E86:E88"/>
+    <mergeCell ref="E89:E91"/>
+    <mergeCell ref="E92:E94"/>
+    <mergeCell ref="E95:E97"/>
+    <mergeCell ref="E98:E100"/>
+    <mergeCell ref="E101:E103"/>
+    <mergeCell ref="E104:E106"/>
+    <mergeCell ref="E107:E109"/>
+    <mergeCell ref="E110:E112"/>
+    <mergeCell ref="E113:E115"/>
     <mergeCell ref="F2:F4"/>
     <mergeCell ref="F5:F7"/>
     <mergeCell ref="F8:F19"/>
@@ -1421,11 +2990,35 @@
     <mergeCell ref="F26:F28"/>
     <mergeCell ref="F29:F31"/>
     <mergeCell ref="F32:F43"/>
+    <mergeCell ref="F44:F46"/>
+    <mergeCell ref="F47:F49"/>
+    <mergeCell ref="F50:F52"/>
+    <mergeCell ref="F53:F55"/>
+    <mergeCell ref="F56:F67"/>
+    <mergeCell ref="F68:F70"/>
+    <mergeCell ref="F71:F73"/>
+    <mergeCell ref="F74:F76"/>
+    <mergeCell ref="F77:F79"/>
+    <mergeCell ref="F80:F91"/>
+    <mergeCell ref="F92:F94"/>
+    <mergeCell ref="F95:F97"/>
+    <mergeCell ref="F98:F100"/>
+    <mergeCell ref="F101:F103"/>
+    <mergeCell ref="F104:F115"/>
     <mergeCell ref="G2:G5"/>
     <mergeCell ref="G6:G21"/>
     <mergeCell ref="G22:G25"/>
     <mergeCell ref="G26:G29"/>
-    <mergeCell ref="G30:G43"/>
+    <mergeCell ref="G30:G45"/>
+    <mergeCell ref="G46:G49"/>
+    <mergeCell ref="G50:G53"/>
+    <mergeCell ref="G54:G69"/>
+    <mergeCell ref="G70:G73"/>
+    <mergeCell ref="G74:G77"/>
+    <mergeCell ref="G78:G93"/>
+    <mergeCell ref="G94:G97"/>
+    <mergeCell ref="G98:G101"/>
+    <mergeCell ref="G102:G115"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix missing guards bug + Finish getting missing guards from table
</commit_message>
<xml_diff>
--- a/watch_list.xlsx
+++ b/watch_list.xlsx
@@ -455,9 +455,9 @@
     <col width="6" customWidth="1" min="1" max="1"/>
     <col width="7" customWidth="1" min="2" max="2"/>
     <col width="18" customWidth="1" min="3" max="3"/>
-    <col width="18" customWidth="1" min="4" max="4"/>
-    <col width="18" customWidth="1" min="5" max="5"/>
-    <col width="19" customWidth="1" min="6" max="6"/>
+    <col width="16" customWidth="1" min="4" max="4"/>
+    <col width="15" customWidth="1" min="5" max="5"/>
+    <col width="16" customWidth="1" min="6" max="6"/>
     <col width="6" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
@@ -497,7 +497,7 @@
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>ה</t>
+          <t>ו</t>
         </is>
       </c>
       <c r="B2" s="3" t="inlineStr">
@@ -507,26 +507,26 @@
       </c>
       <c r="C2" s="3" t="inlineStr">
         <is>
-          <t>דבוש
-פיאצה</t>
+          <t>אבנר
+שגיא</t>
         </is>
       </c>
       <c r="D2" s="3" t="inlineStr">
         <is>
-          <t>אגומס
-דעאל</t>
+          <t>דימה
+שבצוב</t>
         </is>
       </c>
       <c r="E2" s="3" t="inlineStr">
         <is>
-          <t>אלכסיי
-לומיאנסקי</t>
+          <t>אור
+אסרף</t>
         </is>
       </c>
       <c r="F2" s="3" t="inlineStr">
         <is>
-          <t>ארד
-שראל</t>
+          <t>לוטם
+סיני</t>
         </is>
       </c>
       <c r="G2" s="3" t="n"/>
@@ -566,20 +566,20 @@
       </c>
       <c r="C5" s="3" t="inlineStr">
         <is>
-          <t>עמיחי
-לואיס</t>
+          <t>אנזו
+שרעבי</t>
         </is>
       </c>
       <c r="D5" s="3" t="inlineStr">
         <is>
-          <t>קריספין
-רווה</t>
+          <t>דימנטמן
+מטמוני</t>
         </is>
       </c>
       <c r="E5" s="3" t="inlineStr">
         <is>
-          <t>משה
-שמעון</t>
+          <t>דותן
+ליאור</t>
         </is>
       </c>
       <c r="F5" s="3" t="n"/>
@@ -597,9 +597,7 @@
       <c r="E6" s="3" t="n"/>
       <c r="F6" s="3" t="inlineStr">
         <is>
-          <t>נח
-דימנטמן
-מטמוני</t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
       <c r="G6" s="3" t="n"/>
@@ -614,11 +612,7 @@
       <c r="C7" s="3" t="n"/>
       <c r="D7" s="3" t="n"/>
       <c r="E7" s="3" t="n"/>
-      <c r="F7" s="3" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
+      <c r="F7" s="3" t="n"/>
       <c r="G7" s="3" t="n"/>
     </row>
     <row r="8">
@@ -630,20 +624,20 @@
       </c>
       <c r="C8" s="3" t="inlineStr">
         <is>
-          <t>נפמן
-סדון</t>
+          <t>אלכסיי
+לומיאנסקי</t>
         </is>
       </c>
       <c r="D8" s="3" t="inlineStr">
         <is>
-          <t>אסף
-יונג</t>
+          <t>דעאל
+לואיס</t>
         </is>
       </c>
       <c r="E8" s="3" t="inlineStr">
         <is>
-          <t>דורון
-שגיא</t>
+          <t>אנדי
+דוד</t>
         </is>
       </c>
       <c r="F8" s="3" t="n"/>
@@ -684,20 +678,20 @@
       </c>
       <c r="C11" s="3" t="inlineStr">
         <is>
-          <t>דימה
-שבצוב</t>
+          <t>כלפה
+שמעון</t>
         </is>
       </c>
       <c r="D11" s="3" t="inlineStr">
         <is>
-          <t>אור
-אסרף</t>
+          <t>ארד
+יואל</t>
         </is>
       </c>
       <c r="E11" s="3" t="inlineStr">
         <is>
-          <t>איתי כהן
-אבנר</t>
+          <t>נפמן
+סדון</t>
         </is>
       </c>
       <c r="F11" s="3" t="n"/>
@@ -738,20 +732,20 @@
       </c>
       <c r="C14" s="3" t="inlineStr">
         <is>
-          <t>לוטם
-סיני</t>
+          <t>מרדש
+משה</t>
         </is>
       </c>
       <c r="D14" s="3" t="inlineStr">
         <is>
-          <t>אנזו
-שרעבי</t>
+          <t>אסף
+דורון</t>
         </is>
       </c>
       <c r="E14" s="3" t="inlineStr">
         <is>
-          <t>אנדי
-דוד</t>
+          <t>קריספין
+רווה</t>
         </is>
       </c>
       <c r="F14" s="3" t="n"/>
@@ -792,20 +786,20 @@
       </c>
       <c r="C17" s="3" t="inlineStr">
         <is>
-          <t>דותן
-ליאור</t>
+          <t>דבוש
+פיאצה</t>
         </is>
       </c>
       <c r="D17" s="3" t="inlineStr">
         <is>
-          <t>אלכסיי
-לומיאנסקי</t>
+          <t>שראל
+שרעבי</t>
         </is>
       </c>
       <c r="E17" s="3" t="inlineStr">
         <is>
-          <t>לואיס
-דעאל</t>
+          <t>דימה
+שבצוב</t>
         </is>
       </c>
       <c r="F17" s="3" t="n"/>
@@ -846,20 +840,20 @@
       </c>
       <c r="C20" s="3" t="inlineStr">
         <is>
-          <t>דימנטמן
-מטמוני</t>
+          <t>לוטם
+סיני</t>
         </is>
       </c>
       <c r="D20" s="3" t="inlineStr">
         <is>
-          <t>דובר
-כלפה</t>
+          <t>אור
+אסרף</t>
         </is>
       </c>
       <c r="E20" s="3" t="inlineStr">
         <is>
-          <t>ארד
-יואל</t>
+          <t>אבנר
+איתי כהן</t>
         </is>
       </c>
       <c r="F20" s="3" t="n"/>
@@ -890,8 +884,8 @@
       <c r="E22" s="3" t="n"/>
       <c r="F22" s="3" t="inlineStr">
         <is>
-          <t>קריספין
-שמעון</t>
+          <t>דעאל
+לומיאנסקי</t>
         </is>
       </c>
       <c r="G22" s="3" t="n"/>
@@ -905,20 +899,20 @@
       </c>
       <c r="C23" s="3" t="inlineStr">
         <is>
-          <t>נפמן
-סדון</t>
+          <t>שגיא
+ליאור</t>
         </is>
       </c>
       <c r="D23" s="3" t="inlineStr">
         <is>
-          <t>איתי כהן
-לישי</t>
+          <t>אנדי
+דוד</t>
         </is>
       </c>
       <c r="E23" s="3" t="inlineStr">
         <is>
-          <t>דורון
-יונג</t>
+          <t>אנזו
+כלפה</t>
         </is>
       </c>
       <c r="F23" s="3" t="n"/>
@@ -927,7 +921,7 @@
     <row r="24">
       <c r="A24" s="3" t="inlineStr">
         <is>
-          <t>ו</t>
+          <t>שבת</t>
         </is>
       </c>
       <c r="B24" s="3" t="inlineStr">
@@ -963,26 +957,26 @@
       </c>
       <c r="C26" s="3" t="inlineStr">
         <is>
-          <t>אבנר
-שגיא</t>
+          <t>ארד
+יואל</t>
         </is>
       </c>
       <c r="D26" s="3" t="inlineStr">
         <is>
-          <t>דימה
-שבצוב</t>
+          <t>מרדש
+משה</t>
         </is>
       </c>
       <c r="E26" s="3" t="inlineStr">
         <is>
-          <t>אור
-אסרף</t>
+          <t>לואיס
+שמעון</t>
         </is>
       </c>
       <c r="F26" s="3" t="inlineStr">
         <is>
-          <t>לוטם
-סיני</t>
+          <t>נפמן
+סדון</t>
         </is>
       </c>
       <c r="G26" s="3" t="n"/>
@@ -1022,20 +1016,20 @@
       </c>
       <c r="C29" s="3" t="inlineStr">
         <is>
-          <t>אנזו
-שרעבי</t>
+          <t>אסף
+דורון</t>
         </is>
       </c>
       <c r="D29" s="3" t="inlineStr">
         <is>
-          <t>דימנטמן
-מטמוני</t>
+          <t>קריספין
+רווה</t>
         </is>
       </c>
       <c r="E29" s="3" t="inlineStr">
         <is>
-          <t>דותן
-ליאור</t>
+          <t>דבוש
+פיאצה</t>
         </is>
       </c>
       <c r="F29" s="3" t="n"/>
@@ -1080,20 +1074,20 @@
       </c>
       <c r="C32" s="3" t="inlineStr">
         <is>
-          <t>אלכסיי
-לומיאנסקי</t>
+          <t>שראל
+שרעבי</t>
         </is>
       </c>
       <c r="D32" s="3" t="inlineStr">
         <is>
-          <t>דעאל
-לואיס</t>
+          <t>דימה
+שבצוב</t>
         </is>
       </c>
       <c r="E32" s="3" t="inlineStr">
         <is>
-          <t>אנדי
-דוד</t>
+          <t>אור
+אסרף</t>
         </is>
       </c>
       <c r="F32" s="3" t="n"/>
@@ -1134,20 +1128,20 @@
       </c>
       <c r="C35" s="3" t="inlineStr">
         <is>
-          <t>כלפה
-שמעון</t>
+          <t>אבנר
+לומיאנסקי</t>
         </is>
       </c>
       <c r="D35" s="3" t="inlineStr">
         <is>
-          <t>ארד
-יואל</t>
+          <t>איתי כהן
+כלפה</t>
         </is>
       </c>
       <c r="E35" s="3" t="inlineStr">
         <is>
-          <t>נפמן
-סדון</t>
+          <t>לוטם
+סיני</t>
         </is>
       </c>
       <c r="F35" s="3" t="n"/>
@@ -1188,20 +1182,20 @@
       </c>
       <c r="C38" s="3" t="inlineStr">
         <is>
-          <t>מרדש
-משה</t>
+          <t>דעאל
+שגיא</t>
         </is>
       </c>
       <c r="D38" s="3" t="inlineStr">
         <is>
-          <t>אסף
-דורון</t>
+          <t>לואיס
+אנזו</t>
         </is>
       </c>
       <c r="E38" s="3" t="inlineStr">
         <is>
-          <t>קריספין
-רווה</t>
+          <t>אנדי
+דוד</t>
         </is>
       </c>
       <c r="F38" s="3" t="n"/>
@@ -1242,20 +1236,20 @@
       </c>
       <c r="C41" s="3" t="inlineStr">
         <is>
-          <t>דבוש
-פיאצה</t>
+          <t>נפמן
+סדון</t>
         </is>
       </c>
       <c r="D41" s="3" t="inlineStr">
         <is>
-          <t>שראל
-שרעבי</t>
+          <t>ארד
+יואל</t>
         </is>
       </c>
       <c r="E41" s="3" t="inlineStr">
         <is>
-          <t>דימה
-שבצוב</t>
+          <t>ליאור
+משה</t>
         </is>
       </c>
       <c r="F41" s="3" t="n"/>
@@ -1334,7 +1328,7 @@
     <mergeCell ref="E38:E40"/>
     <mergeCell ref="E41:E43"/>
     <mergeCell ref="F2:F5"/>
-    <mergeCell ref="F7:F21"/>
+    <mergeCell ref="F6:F21"/>
     <mergeCell ref="F22:F25"/>
     <mergeCell ref="F26:F29"/>
     <mergeCell ref="F30:F43"/>

</xml_diff>

<commit_message>
Add same ttime partners
</commit_message>
<xml_diff>
--- a/watch_list.xlsx
+++ b/watch_list.xlsx
@@ -456,7 +456,7 @@
     <col width="7" customWidth="1" min="2" max="2"/>
     <col width="18" customWidth="1" min="3" max="3"/>
     <col width="16" customWidth="1" min="4" max="4"/>
-    <col width="15" customWidth="1" min="5" max="5"/>
+    <col width="16" customWidth="1" min="5" max="5"/>
     <col width="16" customWidth="1" min="6" max="6"/>
     <col width="6" customWidth="1" min="7" max="7"/>
   </cols>
@@ -1296,14 +1296,14 @@
       </c>
       <c r="D44" s="3" t="inlineStr">
         <is>
-          <t>דבוש
-פיאצה</t>
+          <t>אור
+דורון</t>
         </is>
       </c>
       <c r="E44" s="3" t="inlineStr">
         <is>
-          <t>אסף
-דורון</t>
+          <t>קריספין
+רווה</t>
         </is>
       </c>
       <c r="F44" s="3" t="n"/>
@@ -1334,8 +1334,8 @@
       <c r="E46" s="3" t="n"/>
       <c r="F46" s="3" t="inlineStr">
         <is>
-          <t>קריספין
-רווה</t>
+          <t>דבוש
+פיאצה</t>
         </is>
       </c>
       <c r="G46" s="3" t="n"/>
@@ -1349,7 +1349,7 @@
       </c>
       <c r="C47" s="3" t="inlineStr">
         <is>
-          <t>אור
+          <t>אסף
 אסרף</t>
         </is>
       </c>
@@ -1407,26 +1407,26 @@
       </c>
       <c r="C50" s="3" t="inlineStr">
         <is>
-          <t>אנזו
-לואיס</t>
-        </is>
-      </c>
-      <c r="D50" s="3" t="inlineStr">
-        <is>
           <t>לוטם
 סיני</t>
         </is>
       </c>
+      <c r="D50" s="3" t="inlineStr">
+        <is>
+          <t>אבנר
+לומיאנסקי</t>
+        </is>
+      </c>
       <c r="E50" s="3" t="inlineStr">
+        <is>
+          <t>דעאל
+שגיא</t>
+        </is>
+      </c>
+      <c r="F50" s="3" t="inlineStr">
         <is>
           <t>איתי כהן
 כלפה</t>
-        </is>
-      </c>
-      <c r="F50" s="3" t="inlineStr">
-        <is>
-          <t>אבנר
-דעאל</t>
         </is>
       </c>
       <c r="G50" s="3" t="n"/>
@@ -1466,14 +1466,14 @@
       </c>
       <c r="C53" s="3" t="inlineStr">
         <is>
+          <t>אנזו
+לואיס</t>
+        </is>
+      </c>
+      <c r="D53" s="3" t="inlineStr">
+        <is>
           <t>אנדי
 דוד</t>
-        </is>
-      </c>
-      <c r="D53" s="3" t="inlineStr">
-        <is>
-          <t>לומיאנסקי
-שגיא</t>
         </is>
       </c>
       <c r="E53" s="3" t="inlineStr">
@@ -1524,8 +1524,8 @@
       </c>
       <c r="C56" s="3" t="inlineStr">
         <is>
-          <t>דבוש
-פיאצה</t>
+          <t>ארד
+יואל</t>
         </is>
       </c>
       <c r="D56" s="3" t="inlineStr">
@@ -1536,8 +1536,8 @@
       </c>
       <c r="E56" s="3" t="inlineStr">
         <is>
-          <t>ארד
-יואל</t>
+          <t>דורון
+שמעון</t>
         </is>
       </c>
       <c r="F56" s="3" t="n"/>
@@ -1578,20 +1578,20 @@
       </c>
       <c r="C59" s="3" t="inlineStr">
         <is>
-          <t>אסף
-דורון</t>
-        </is>
-      </c>
-      <c r="D59" s="3" t="inlineStr">
-        <is>
-          <t>מרדש
-שמעון</t>
-        </is>
-      </c>
-      <c r="E59" s="3" t="inlineStr">
-        <is>
           <t>קריספין
 רווה</t>
+        </is>
+      </c>
+      <c r="D59" s="3" t="inlineStr">
+        <is>
+          <t>דבוש
+פיאצה</t>
+        </is>
+      </c>
+      <c r="E59" s="3" t="inlineStr">
+        <is>
+          <t>אור
+מרדש</t>
         </is>
       </c>
       <c r="F59" s="3" t="n"/>
@@ -1632,20 +1632,20 @@
       </c>
       <c r="C62" s="3" t="inlineStr">
         <is>
-          <t>דותן
-ניסנוב</t>
-        </is>
-      </c>
-      <c r="D62" s="3" t="inlineStr">
-        <is>
-          <t>אור
-אסרף</t>
-        </is>
-      </c>
-      <c r="E62" s="3" t="inlineStr">
-        <is>
           <t>שראל
 שרעבי</t>
+        </is>
+      </c>
+      <c r="D62" s="3" t="inlineStr">
+        <is>
+          <t>יונג
+ניסנוב</t>
+        </is>
+      </c>
+      <c r="E62" s="3" t="inlineStr">
+        <is>
+          <t>דימנטמן
+מטמוני</t>
         </is>
       </c>
       <c r="F62" s="3" t="n"/>
@@ -1692,14 +1692,14 @@
       </c>
       <c r="D65" s="3" t="inlineStr">
         <is>
-          <t>דובר
-כלפה</t>
+          <t>דותן
+שגיא</t>
         </is>
       </c>
       <c r="E65" s="3" t="inlineStr">
         <is>
-          <t>לוטם
-סיני</t>
+          <t>אסף
+אסרף</t>
         </is>
       </c>
       <c r="F65" s="3" t="n"/>

</xml_diff>

<commit_message>
Add toranout + conenout
</commit_message>
<xml_diff>
--- a/watch_list.xlsx
+++ b/watch_list.xlsx
@@ -444,7 +444,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G67"/>
+  <dimension ref="A1:H67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,11 +454,12 @@
   <cols>
     <col width="6" customWidth="1" min="1" max="1"/>
     <col width="7" customWidth="1" min="2" max="2"/>
-    <col width="18" customWidth="1" min="3" max="3"/>
-    <col width="16" customWidth="1" min="4" max="4"/>
-    <col width="16" customWidth="1" min="5" max="5"/>
-    <col width="16" customWidth="1" min="6" max="6"/>
-    <col width="6" customWidth="1" min="7" max="7"/>
+    <col width="17" customWidth="1" min="3" max="3"/>
+    <col width="18" customWidth="1" min="4" max="4"/>
+    <col width="17" customWidth="1" min="5" max="5"/>
+    <col width="20" customWidth="1" min="6" max="6"/>
+    <col width="12" customWidth="1" min="7" max="7"/>
+    <col width="6" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -492,7 +493,12 @@
           <t>פטרול</t>
         </is>
       </c>
-      <c r="G1" s="3" t="n"/>
+      <c r="G1" s="2" t="inlineStr">
+        <is>
+          <t>כתת כוננות</t>
+        </is>
+      </c>
+      <c r="H1" s="3" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
@@ -507,29 +513,34 @@
       </c>
       <c r="C2" s="3" t="inlineStr">
         <is>
+          <t>אסרף
+יונג</t>
+        </is>
+      </c>
+      <c r="D2" s="3" t="inlineStr">
+        <is>
+          <t>דורון
+שגיא</t>
+        </is>
+      </c>
+      <c r="E2" s="3" t="inlineStr">
+        <is>
           <t>אבנר
-שגיא</t>
-        </is>
-      </c>
-      <c r="D2" s="3" t="inlineStr">
-        <is>
-          <t>דימה
-שבצוב</t>
-        </is>
-      </c>
-      <c r="E2" s="3" t="inlineStr">
-        <is>
-          <t>אור
-אסרף</t>
+ליאור</t>
         </is>
       </c>
       <c r="F2" s="3" t="inlineStr">
         <is>
-          <t>לוטם
-סיני</t>
-        </is>
-      </c>
-      <c r="G2" s="3" t="n"/>
+          <t>ארד
+יואל</t>
+        </is>
+      </c>
+      <c r="G2" s="3" t="inlineStr">
+        <is>
+          <t>11 חדר</t>
+        </is>
+      </c>
+      <c r="H2" s="3" t="n"/>
     </row>
     <row r="3">
       <c r="A3" s="3" t="n"/>
@@ -543,6 +554,7 @@
       <c r="E3" s="3" t="n"/>
       <c r="F3" s="3" t="n"/>
       <c r="G3" s="3" t="n"/>
+      <c r="H3" s="3" t="n"/>
     </row>
     <row r="4">
       <c r="A4" s="3" t="n"/>
@@ -556,6 +568,7 @@
       <c r="E4" s="3" t="n"/>
       <c r="F4" s="3" t="n"/>
       <c r="G4" s="3" t="n"/>
+      <c r="H4" s="3" t="n"/>
     </row>
     <row r="5">
       <c r="A5" s="3" t="n"/>
@@ -566,24 +579,25 @@
       </c>
       <c r="C5" s="3" t="inlineStr">
         <is>
-          <t>אנזו
-שרעבי</t>
-        </is>
-      </c>
-      <c r="D5" s="3" t="inlineStr">
-        <is>
           <t>דימנטמן
 מטמוני</t>
         </is>
       </c>
+      <c r="D5" s="3" t="inlineStr">
+        <is>
+          <t>אנזו
+לואיס</t>
+        </is>
+      </c>
       <c r="E5" s="3" t="inlineStr">
         <is>
-          <t>דותן
-ליאור</t>
+          <t>אנדי
+דוד</t>
         </is>
       </c>
       <c r="F5" s="3" t="n"/>
       <c r="G5" s="3" t="n"/>
+      <c r="H5" s="3" t="n"/>
     </row>
     <row r="6">
       <c r="A6" s="3" t="n"/>
@@ -597,10 +611,11 @@
       <c r="E6" s="3" t="n"/>
       <c r="F6" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t>5 תורני רס"פ - חדר</t>
         </is>
       </c>
       <c r="G6" s="3" t="n"/>
+      <c r="H6" s="3" t="n"/>
     </row>
     <row r="7">
       <c r="A7" s="3" t="n"/>
@@ -614,6 +629,7 @@
       <c r="E7" s="3" t="n"/>
       <c r="F7" s="3" t="n"/>
       <c r="G7" s="3" t="n"/>
+      <c r="H7" s="3" t="n"/>
     </row>
     <row r="8">
       <c r="A8" s="3" t="n"/>
@@ -624,24 +640,29 @@
       </c>
       <c r="C8" s="3" t="inlineStr">
         <is>
+          <t>כלפה
+ניסנוב</t>
+        </is>
+      </c>
+      <c r="D8" s="3" t="inlineStr">
+        <is>
           <t>אלכסיי
 לומיאנסקי</t>
         </is>
       </c>
-      <c r="D8" s="3" t="inlineStr">
-        <is>
-          <t>דעאל
-לואיס</t>
-        </is>
-      </c>
       <c r="E8" s="3" t="inlineStr">
         <is>
-          <t>אנדי
-דוד</t>
+          <t>אגומס
+דעאל</t>
         </is>
       </c>
       <c r="F8" s="3" t="n"/>
-      <c r="G8" s="3" t="n"/>
+      <c r="G8" s="3" t="inlineStr">
+        <is>
+          <t>9 חדר</t>
+        </is>
+      </c>
+      <c r="H8" s="3" t="n"/>
     </row>
     <row r="9">
       <c r="A9" s="3" t="n"/>
@@ -655,6 +676,7 @@
       <c r="E9" s="3" t="n"/>
       <c r="F9" s="3" t="n"/>
       <c r="G9" s="3" t="n"/>
+      <c r="H9" s="3" t="n"/>
     </row>
     <row r="10">
       <c r="A10" s="3" t="n"/>
@@ -668,6 +690,7 @@
       <c r="E10" s="3" t="n"/>
       <c r="F10" s="3" t="n"/>
       <c r="G10" s="3" t="n"/>
+      <c r="H10" s="3" t="n"/>
     </row>
     <row r="11">
       <c r="A11" s="3" t="n"/>
@@ -678,24 +701,25 @@
       </c>
       <c r="C11" s="3" t="inlineStr">
         <is>
-          <t>כלפה
+          <t>קריספין
 שמעון</t>
         </is>
       </c>
       <c r="D11" s="3" t="inlineStr">
         <is>
-          <t>ארד
-יואל</t>
+          <t>דימה
+שבצוב</t>
         </is>
       </c>
       <c r="E11" s="3" t="inlineStr">
         <is>
-          <t>נפמן
-סדון</t>
+          <t>איתי כהן
+שרעבי</t>
         </is>
       </c>
       <c r="F11" s="3" t="n"/>
       <c r="G11" s="3" t="n"/>
+      <c r="H11" s="3" t="n"/>
     </row>
     <row r="12">
       <c r="A12" s="3" t="n"/>
@@ -709,6 +733,7 @@
       <c r="E12" s="3" t="n"/>
       <c r="F12" s="3" t="n"/>
       <c r="G12" s="3" t="n"/>
+      <c r="H12" s="3" t="n"/>
     </row>
     <row r="13">
       <c r="A13" s="3" t="n"/>
@@ -722,6 +747,7 @@
       <c r="E13" s="3" t="n"/>
       <c r="F13" s="3" t="n"/>
       <c r="G13" s="3" t="n"/>
+      <c r="H13" s="3" t="n"/>
     </row>
     <row r="14">
       <c r="A14" s="3" t="n"/>
@@ -732,24 +758,29 @@
       </c>
       <c r="C14" s="3" t="inlineStr">
         <is>
-          <t>מרדש
-משה</t>
+          <t>לוטם
+סיני</t>
         </is>
       </c>
       <c r="D14" s="3" t="inlineStr">
         <is>
-          <t>אסף
-דורון</t>
+          <t>משה
+רווה</t>
         </is>
       </c>
       <c r="E14" s="3" t="inlineStr">
         <is>
-          <t>קריספין
-רווה</t>
+          <t>נפמן
+סדון</t>
         </is>
       </c>
       <c r="F14" s="3" t="n"/>
-      <c r="G14" s="3" t="n"/>
+      <c r="G14" s="3" t="inlineStr">
+        <is>
+          <t>8 חדר</t>
+        </is>
+      </c>
+      <c r="H14" s="3" t="n"/>
     </row>
     <row r="15">
       <c r="A15" s="3" t="n"/>
@@ -763,6 +794,7 @@
       <c r="E15" s="3" t="n"/>
       <c r="F15" s="3" t="n"/>
       <c r="G15" s="3" t="n"/>
+      <c r="H15" s="3" t="n"/>
     </row>
     <row r="16">
       <c r="A16" s="3" t="n"/>
@@ -776,6 +808,7 @@
       <c r="E16" s="3" t="n"/>
       <c r="F16" s="3" t="n"/>
       <c r="G16" s="3" t="n"/>
+      <c r="H16" s="3" t="n"/>
     </row>
     <row r="17">
       <c r="A17" s="3" t="n"/>
@@ -786,24 +819,25 @@
       </c>
       <c r="C17" s="3" t="inlineStr">
         <is>
+          <t>ארד
+יואל</t>
+        </is>
+      </c>
+      <c r="D17" s="3" t="inlineStr">
+        <is>
           <t>דבוש
 פיאצה</t>
         </is>
       </c>
-      <c r="D17" s="3" t="inlineStr">
-        <is>
-          <t>שראל
-שרעבי</t>
-        </is>
-      </c>
       <c r="E17" s="3" t="inlineStr">
         <is>
-          <t>דימה
-שבצוב</t>
+          <t>אור
+שראל</t>
         </is>
       </c>
       <c r="F17" s="3" t="n"/>
       <c r="G17" s="3" t="n"/>
+      <c r="H17" s="3" t="n"/>
     </row>
     <row r="18">
       <c r="A18" s="3" t="n"/>
@@ -817,6 +851,7 @@
       <c r="E18" s="3" t="n"/>
       <c r="F18" s="3" t="n"/>
       <c r="G18" s="3" t="n"/>
+      <c r="H18" s="3" t="n"/>
     </row>
     <row r="19">
       <c r="A19" s="3" t="n"/>
@@ -830,6 +865,7 @@
       <c r="E19" s="3" t="n"/>
       <c r="F19" s="3" t="n"/>
       <c r="G19" s="3" t="n"/>
+      <c r="H19" s="3" t="n"/>
     </row>
     <row r="20">
       <c r="A20" s="3" t="n"/>
@@ -840,24 +876,29 @@
       </c>
       <c r="C20" s="3" t="inlineStr">
         <is>
-          <t>לוטם
-סיני</t>
+          <t>אנזו
+שגיא</t>
         </is>
       </c>
       <c r="D20" s="3" t="inlineStr">
         <is>
-          <t>אור
-אסרף</t>
+          <t>אבנר
+ליאור</t>
         </is>
       </c>
       <c r="E20" s="3" t="inlineStr">
         <is>
-          <t>אבנר
-איתי כהן</t>
+          <t>דורון
+מרדש</t>
         </is>
       </c>
       <c r="F20" s="3" t="n"/>
-      <c r="G20" s="3" t="n"/>
+      <c r="G20" s="3" t="inlineStr">
+        <is>
+          <t>10 חדר</t>
+        </is>
+      </c>
+      <c r="H20" s="3" t="n"/>
     </row>
     <row r="21">
       <c r="A21" s="3" t="n"/>
@@ -871,6 +912,7 @@
       <c r="E21" s="3" t="n"/>
       <c r="F21" s="3" t="n"/>
       <c r="G21" s="3" t="n"/>
+      <c r="H21" s="3" t="n"/>
     </row>
     <row r="22">
       <c r="A22" s="3" t="n"/>
@@ -884,11 +926,12 @@
       <c r="E22" s="3" t="n"/>
       <c r="F22" s="3" t="inlineStr">
         <is>
-          <t>דעאל
-לומיאנסקי</t>
+          <t>אנדי
+דוד</t>
         </is>
       </c>
       <c r="G22" s="3" t="n"/>
+      <c r="H22" s="3" t="n"/>
     </row>
     <row r="23">
       <c r="A23" s="3" t="n"/>
@@ -899,24 +942,25 @@
       </c>
       <c r="C23" s="3" t="inlineStr">
         <is>
-          <t>שגיא
-ליאור</t>
+          <t>לואיס
+לומיאנסקי</t>
         </is>
       </c>
       <c r="D23" s="3" t="inlineStr">
         <is>
-          <t>אנדי
-דוד</t>
+          <t>דעאל
+כלפה</t>
         </is>
       </c>
       <c r="E23" s="3" t="inlineStr">
         <is>
-          <t>אנזו
-כלפה</t>
+          <t>אסף
+אסרף</t>
         </is>
       </c>
       <c r="F23" s="3" t="n"/>
       <c r="G23" s="3" t="n"/>
+      <c r="H23" s="3" t="n"/>
     </row>
     <row r="24">
       <c r="A24" s="3" t="inlineStr">
@@ -934,6 +978,7 @@
       <c r="E24" s="3" t="n"/>
       <c r="F24" s="3" t="n"/>
       <c r="G24" s="3" t="n"/>
+      <c r="H24" s="3" t="n"/>
     </row>
     <row r="25">
       <c r="A25" s="3" t="n"/>
@@ -947,6 +992,7 @@
       <c r="E25" s="3" t="n"/>
       <c r="F25" s="3" t="n"/>
       <c r="G25" s="3" t="n"/>
+      <c r="H25" s="3" t="n"/>
     </row>
     <row r="26">
       <c r="A26" s="3" t="n"/>
@@ -957,29 +1003,34 @@
       </c>
       <c r="C26" s="3" t="inlineStr">
         <is>
-          <t>ארד
-יואל</t>
+          <t>שראל
+שרעבי</t>
         </is>
       </c>
       <c r="D26" s="3" t="inlineStr">
         <is>
-          <t>מרדש
-משה</t>
+          <t>קריספין
+רווה</t>
         </is>
       </c>
       <c r="E26" s="3" t="inlineStr">
         <is>
-          <t>לואיס
+          <t>דימה
+שבצוב</t>
+        </is>
+      </c>
+      <c r="F26" s="3" t="inlineStr">
+        <is>
+          <t>איתי כהן
 שמעון</t>
         </is>
       </c>
-      <c r="F26" s="3" t="inlineStr">
-        <is>
-          <t>נפמן
-סדון</t>
-        </is>
-      </c>
-      <c r="G26" s="3" t="n"/>
+      <c r="G26" s="3" t="inlineStr">
+        <is>
+          <t>6 חדר</t>
+        </is>
+      </c>
+      <c r="H26" s="3" t="n"/>
     </row>
     <row r="27">
       <c r="A27" s="3" t="n"/>
@@ -993,6 +1044,7 @@
       <c r="E27" s="3" t="n"/>
       <c r="F27" s="3" t="n"/>
       <c r="G27" s="3" t="n"/>
+      <c r="H27" s="3" t="n"/>
     </row>
     <row r="28">
       <c r="A28" s="3" t="n"/>
@@ -1006,6 +1058,7 @@
       <c r="E28" s="3" t="n"/>
       <c r="F28" s="3" t="n"/>
       <c r="G28" s="3" t="n"/>
+      <c r="H28" s="3" t="n"/>
     </row>
     <row r="29">
       <c r="A29" s="3" t="n"/>
@@ -1016,24 +1069,25 @@
       </c>
       <c r="C29" s="3" t="inlineStr">
         <is>
-          <t>אסף
-דורון</t>
-        </is>
-      </c>
-      <c r="D29" s="3" t="inlineStr">
-        <is>
-          <t>קריספין
-רווה</t>
-        </is>
-      </c>
-      <c r="E29" s="3" t="inlineStr">
-        <is>
           <t>דבוש
 פיאצה</t>
         </is>
       </c>
+      <c r="D29" s="3" t="inlineStr">
+        <is>
+          <t>נפמן
+סדון</t>
+        </is>
+      </c>
+      <c r="E29" s="3" t="inlineStr">
+        <is>
+          <t>לוטם
+סיני</t>
+        </is>
+      </c>
       <c r="F29" s="3" t="n"/>
       <c r="G29" s="3" t="n"/>
+      <c r="H29" s="3" t="n"/>
     </row>
     <row r="30">
       <c r="A30" s="3" t="n"/>
@@ -1047,10 +1101,11 @@
       <c r="E30" s="3" t="n"/>
       <c r="F30" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t>6 תורני רס"פ - חדר</t>
         </is>
       </c>
       <c r="G30" s="3" t="n"/>
+      <c r="H30" s="3" t="n"/>
     </row>
     <row r="31">
       <c r="A31" s="3" t="n"/>
@@ -1064,6 +1119,7 @@
       <c r="E31" s="3" t="n"/>
       <c r="F31" s="3" t="n"/>
       <c r="G31" s="3" t="n"/>
+      <c r="H31" s="3" t="n"/>
     </row>
     <row r="32">
       <c r="A32" s="3" t="n"/>
@@ -1074,24 +1130,29 @@
       </c>
       <c r="C32" s="3" t="inlineStr">
         <is>
-          <t>שראל
-שרעבי</t>
+          <t>אבנר
+ליאור</t>
         </is>
       </c>
       <c r="D32" s="3" t="inlineStr">
         <is>
-          <t>דימה
-שבצוב</t>
+          <t>אור
+מרדש</t>
         </is>
       </c>
       <c r="E32" s="3" t="inlineStr">
         <is>
-          <t>אור
-אסרף</t>
+          <t>ארד
+יואל</t>
         </is>
       </c>
       <c r="F32" s="3" t="n"/>
-      <c r="G32" s="3" t="n"/>
+      <c r="G32" s="3" t="inlineStr">
+        <is>
+          <t>5 חדר</t>
+        </is>
+      </c>
+      <c r="H32" s="3" t="n"/>
     </row>
     <row r="33">
       <c r="A33" s="3" t="n"/>
@@ -1105,6 +1166,7 @@
       <c r="E33" s="3" t="n"/>
       <c r="F33" s="3" t="n"/>
       <c r="G33" s="3" t="n"/>
+      <c r="H33" s="3" t="n"/>
     </row>
     <row r="34">
       <c r="A34" s="3" t="n"/>
@@ -1118,6 +1180,7 @@
       <c r="E34" s="3" t="n"/>
       <c r="F34" s="3" t="n"/>
       <c r="G34" s="3" t="n"/>
+      <c r="H34" s="3" t="n"/>
     </row>
     <row r="35">
       <c r="A35" s="3" t="n"/>
@@ -1128,24 +1191,25 @@
       </c>
       <c r="C35" s="3" t="inlineStr">
         <is>
-          <t>אבנר
-לומיאנסקי</t>
+          <t>אסף
+אסרף</t>
         </is>
       </c>
       <c r="D35" s="3" t="inlineStr">
         <is>
-          <t>איתי כהן
-כלפה</t>
+          <t>דורון
+שגיא</t>
         </is>
       </c>
       <c r="E35" s="3" t="inlineStr">
         <is>
-          <t>לוטם
-סיני</t>
+          <t>אנדי
+דוד</t>
         </is>
       </c>
       <c r="F35" s="3" t="n"/>
       <c r="G35" s="3" t="n"/>
+      <c r="H35" s="3" t="n"/>
     </row>
     <row r="36">
       <c r="A36" s="3" t="n"/>
@@ -1159,6 +1223,7 @@
       <c r="E36" s="3" t="n"/>
       <c r="F36" s="3" t="n"/>
       <c r="G36" s="3" t="n"/>
+      <c r="H36" s="3" t="n"/>
     </row>
     <row r="37">
       <c r="A37" s="3" t="n"/>
@@ -1172,6 +1237,7 @@
       <c r="E37" s="3" t="n"/>
       <c r="F37" s="3" t="n"/>
       <c r="G37" s="3" t="n"/>
+      <c r="H37" s="3" t="n"/>
     </row>
     <row r="38">
       <c r="A38" s="3" t="n"/>
@@ -1183,23 +1249,28 @@
       <c r="C38" s="3" t="inlineStr">
         <is>
           <t>דעאל
-שגיא</t>
+כלפה</t>
         </is>
       </c>
       <c r="D38" s="3" t="inlineStr">
         <is>
           <t>לואיס
-אנזו</t>
+לומיאנסקי</t>
         </is>
       </c>
       <c r="E38" s="3" t="inlineStr">
         <is>
-          <t>אנדי
-דוד</t>
+          <t>אנזו
+משה</t>
         </is>
       </c>
       <c r="F38" s="3" t="n"/>
-      <c r="G38" s="3" t="n"/>
+      <c r="G38" s="3" t="inlineStr">
+        <is>
+          <t>11 חדר</t>
+        </is>
+      </c>
+      <c r="H38" s="3" t="n"/>
     </row>
     <row r="39">
       <c r="A39" s="3" t="n"/>
@@ -1213,6 +1284,7 @@
       <c r="E39" s="3" t="n"/>
       <c r="F39" s="3" t="n"/>
       <c r="G39" s="3" t="n"/>
+      <c r="H39" s="3" t="n"/>
     </row>
     <row r="40">
       <c r="A40" s="3" t="n"/>
@@ -1226,6 +1298,7 @@
       <c r="E40" s="3" t="n"/>
       <c r="F40" s="3" t="n"/>
       <c r="G40" s="3" t="n"/>
+      <c r="H40" s="3" t="n"/>
     </row>
     <row r="41">
       <c r="A41" s="3" t="n"/>
@@ -1236,24 +1309,25 @@
       </c>
       <c r="C41" s="3" t="inlineStr">
         <is>
-          <t>נפמן
-סדון</t>
+          <t>איתי כהן
+שמעון</t>
         </is>
       </c>
       <c r="D41" s="3" t="inlineStr">
         <is>
-          <t>ארד
-יואל</t>
+          <t>דבוש
+פיאצה</t>
         </is>
       </c>
       <c r="E41" s="3" t="inlineStr">
         <is>
-          <t>ליאור
-משה</t>
+          <t>שראל
+שרעבי</t>
         </is>
       </c>
       <c r="F41" s="3" t="n"/>
       <c r="G41" s="3" t="n"/>
+      <c r="H41" s="3" t="n"/>
     </row>
     <row r="42">
       <c r="A42" s="3" t="n"/>
@@ -1267,6 +1341,7 @@
       <c r="E42" s="3" t="n"/>
       <c r="F42" s="3" t="n"/>
       <c r="G42" s="3" t="n"/>
+      <c r="H42" s="3" t="n"/>
     </row>
     <row r="43">
       <c r="A43" s="3" t="n"/>
@@ -1280,6 +1355,7 @@
       <c r="E43" s="3" t="n"/>
       <c r="F43" s="3" t="n"/>
       <c r="G43" s="3" t="n"/>
+      <c r="H43" s="3" t="n"/>
     </row>
     <row r="44">
       <c r="A44" s="3" t="n"/>
@@ -1290,14 +1366,14 @@
       </c>
       <c r="C44" s="3" t="inlineStr">
         <is>
-          <t>מרדש
-שמעון</t>
+          <t>נפמן
+סדון</t>
         </is>
       </c>
       <c r="D44" s="3" t="inlineStr">
         <is>
-          <t>אור
-דורון</t>
+          <t>דימה
+שבצוב</t>
         </is>
       </c>
       <c r="E44" s="3" t="inlineStr">
@@ -1307,7 +1383,12 @@
         </is>
       </c>
       <c r="F44" s="3" t="n"/>
-      <c r="G44" s="3" t="n"/>
+      <c r="G44" s="3" t="inlineStr">
+        <is>
+          <t>7 חדר</t>
+        </is>
+      </c>
+      <c r="H44" s="3" t="n"/>
     </row>
     <row r="45">
       <c r="A45" s="3" t="n"/>
@@ -1321,6 +1402,7 @@
       <c r="E45" s="3" t="n"/>
       <c r="F45" s="3" t="n"/>
       <c r="G45" s="3" t="n"/>
+      <c r="H45" s="3" t="n"/>
     </row>
     <row r="46">
       <c r="A46" s="3" t="n"/>
@@ -1334,11 +1416,12 @@
       <c r="E46" s="3" t="n"/>
       <c r="F46" s="3" t="inlineStr">
         <is>
-          <t>דבוש
-פיאצה</t>
+          <t>לוטם
+סיני</t>
         </is>
       </c>
       <c r="G46" s="3" t="n"/>
+      <c r="H46" s="3" t="n"/>
     </row>
     <row r="47">
       <c r="A47" s="3" t="n"/>
@@ -1349,24 +1432,25 @@
       </c>
       <c r="C47" s="3" t="inlineStr">
         <is>
-          <t>אסף
-אסרף</t>
+          <t>ארד
+יואל</t>
         </is>
       </c>
       <c r="D47" s="3" t="inlineStr">
         <is>
-          <t>שראל
-שרעבי</t>
+          <t>אבנר
+ליאור</t>
         </is>
       </c>
       <c r="E47" s="3" t="inlineStr">
         <is>
-          <t>דימה
-שבצוב</t>
+          <t>אור
+מרדש</t>
         </is>
       </c>
       <c r="F47" s="3" t="n"/>
       <c r="G47" s="3" t="n"/>
+      <c r="H47" s="3" t="n"/>
     </row>
     <row r="48">
       <c r="A48" s="3" t="inlineStr">
@@ -1384,6 +1468,7 @@
       <c r="E48" s="3" t="n"/>
       <c r="F48" s="3" t="n"/>
       <c r="G48" s="3" t="n"/>
+      <c r="H48" s="3" t="n"/>
     </row>
     <row r="49">
       <c r="A49" s="3" t="n"/>
@@ -1397,6 +1482,7 @@
       <c r="E49" s="3" t="n"/>
       <c r="F49" s="3" t="n"/>
       <c r="G49" s="3" t="n"/>
+      <c r="H49" s="3" t="n"/>
     </row>
     <row r="50">
       <c r="A50" s="3" t="n"/>
@@ -1407,14 +1493,14 @@
       </c>
       <c r="C50" s="3" t="inlineStr">
         <is>
-          <t>לוטם
-סיני</t>
+          <t>אנדי
+דוד</t>
         </is>
       </c>
       <c r="D50" s="3" t="inlineStr">
         <is>
-          <t>אבנר
-לומיאנסקי</t>
+          <t>אסף
+אסרף</t>
         </is>
       </c>
       <c r="E50" s="3" t="inlineStr">
@@ -1425,11 +1511,16 @@
       </c>
       <c r="F50" s="3" t="inlineStr">
         <is>
-          <t>איתי כהן
-כלפה</t>
-        </is>
-      </c>
-      <c r="G50" s="3" t="n"/>
+          <t>דורון
+משה</t>
+        </is>
+      </c>
+      <c r="G50" s="3" t="inlineStr">
+        <is>
+          <t>9 חדר</t>
+        </is>
+      </c>
+      <c r="H50" s="3" t="n"/>
     </row>
     <row r="51">
       <c r="A51" s="3" t="n"/>
@@ -1443,6 +1534,7 @@
       <c r="E51" s="3" t="n"/>
       <c r="F51" s="3" t="n"/>
       <c r="G51" s="3" t="n"/>
+      <c r="H51" s="3" t="n"/>
     </row>
     <row r="52">
       <c r="A52" s="3" t="n"/>
@@ -1456,6 +1548,7 @@
       <c r="E52" s="3" t="n"/>
       <c r="F52" s="3" t="n"/>
       <c r="G52" s="3" t="n"/>
+      <c r="H52" s="3" t="n"/>
     </row>
     <row r="53">
       <c r="A53" s="3" t="n"/>
@@ -1466,24 +1559,25 @@
       </c>
       <c r="C53" s="3" t="inlineStr">
         <is>
+          <t>דבוש
+פיאצה</t>
+        </is>
+      </c>
+      <c r="D53" s="3" t="inlineStr">
+        <is>
           <t>אנזו
-לואיס</t>
-        </is>
-      </c>
-      <c r="D53" s="3" t="inlineStr">
-        <is>
-          <t>אנדי
-דוד</t>
+כלפה</t>
         </is>
       </c>
       <c r="E53" s="3" t="inlineStr">
         <is>
-          <t>נפמן
-סדון</t>
+          <t>לואיס
+לומיאנסקי</t>
         </is>
       </c>
       <c r="F53" s="3" t="n"/>
       <c r="G53" s="3" t="n"/>
+      <c r="H53" s="3" t="n"/>
     </row>
     <row r="54">
       <c r="A54" s="3" t="n"/>
@@ -1497,10 +1591,11 @@
       <c r="E54" s="3" t="n"/>
       <c r="F54" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t>7 תורני רס"פ - חדר</t>
         </is>
       </c>
       <c r="G54" s="3" t="n"/>
+      <c r="H54" s="3" t="n"/>
     </row>
     <row r="55">
       <c r="A55" s="3" t="n"/>
@@ -1514,6 +1609,7 @@
       <c r="E55" s="3" t="n"/>
       <c r="F55" s="3" t="n"/>
       <c r="G55" s="3" t="n"/>
+      <c r="H55" s="3" t="n"/>
     </row>
     <row r="56">
       <c r="A56" s="3" t="n"/>
@@ -1524,24 +1620,29 @@
       </c>
       <c r="C56" s="3" t="inlineStr">
         <is>
-          <t>ארד
-יואל</t>
+          <t>קריספין
+רווה</t>
         </is>
       </c>
       <c r="D56" s="3" t="inlineStr">
         <is>
-          <t>ליאור
-משה</t>
+          <t>שראל
+שרעבי</t>
         </is>
       </c>
       <c r="E56" s="3" t="inlineStr">
         <is>
-          <t>דורון
+          <t>איתי כהן
 שמעון</t>
         </is>
       </c>
       <c r="F56" s="3" t="n"/>
-      <c r="G56" s="3" t="n"/>
+      <c r="G56" s="3" t="inlineStr">
+        <is>
+          <t>10 חדר</t>
+        </is>
+      </c>
+      <c r="H56" s="3" t="n"/>
     </row>
     <row r="57">
       <c r="A57" s="3" t="n"/>
@@ -1555,6 +1656,7 @@
       <c r="E57" s="3" t="n"/>
       <c r="F57" s="3" t="n"/>
       <c r="G57" s="3" t="n"/>
+      <c r="H57" s="3" t="n"/>
     </row>
     <row r="58">
       <c r="A58" s="3" t="n"/>
@@ -1568,6 +1670,7 @@
       <c r="E58" s="3" t="n"/>
       <c r="F58" s="3" t="n"/>
       <c r="G58" s="3" t="n"/>
+      <c r="H58" s="3" t="n"/>
     </row>
     <row r="59">
       <c r="A59" s="3" t="n"/>
@@ -1578,24 +1681,25 @@
       </c>
       <c r="C59" s="3" t="inlineStr">
         <is>
-          <t>קריספין
-רווה</t>
+          <t>ליאור
+מרדש</t>
         </is>
       </c>
       <c r="D59" s="3" t="inlineStr">
         <is>
-          <t>דבוש
-פיאצה</t>
+          <t>לוטם
+סיני</t>
         </is>
       </c>
       <c r="E59" s="3" t="inlineStr">
         <is>
-          <t>אור
-מרדש</t>
+          <t>דימה
+שבצוב</t>
         </is>
       </c>
       <c r="F59" s="3" t="n"/>
       <c r="G59" s="3" t="n"/>
+      <c r="H59" s="3" t="n"/>
     </row>
     <row r="60">
       <c r="A60" s="3" t="n"/>
@@ -1609,6 +1713,7 @@
       <c r="E60" s="3" t="n"/>
       <c r="F60" s="3" t="n"/>
       <c r="G60" s="3" t="n"/>
+      <c r="H60" s="3" t="n"/>
     </row>
     <row r="61">
       <c r="A61" s="3" t="n"/>
@@ -1622,6 +1727,7 @@
       <c r="E61" s="3" t="n"/>
       <c r="F61" s="3" t="n"/>
       <c r="G61" s="3" t="n"/>
+      <c r="H61" s="3" t="n"/>
     </row>
     <row r="62">
       <c r="A62" s="3" t="n"/>
@@ -1632,24 +1738,29 @@
       </c>
       <c r="C62" s="3" t="inlineStr">
         <is>
-          <t>שראל
-שרעבי</t>
+          <t>דותן
+עמיחי</t>
         </is>
       </c>
       <c r="D62" s="3" t="inlineStr">
-        <is>
-          <t>יונג
-ניסנוב</t>
-        </is>
-      </c>
-      <c r="E62" s="3" t="inlineStr">
         <is>
           <t>דימנטמן
 מטמוני</t>
         </is>
       </c>
+      <c r="E62" s="3" t="inlineStr">
+        <is>
+          <t>יונג
+סדון</t>
+        </is>
+      </c>
       <c r="F62" s="3" t="n"/>
-      <c r="G62" s="3" t="n"/>
+      <c r="G62" s="3" t="inlineStr">
+        <is>
+          <t>8 חדר</t>
+        </is>
+      </c>
+      <c r="H62" s="3" t="n"/>
     </row>
     <row r="63">
       <c r="A63" s="3" t="n"/>
@@ -1663,6 +1774,7 @@
       <c r="E63" s="3" t="n"/>
       <c r="F63" s="3" t="n"/>
       <c r="G63" s="3" t="n"/>
+      <c r="H63" s="3" t="n"/>
     </row>
     <row r="64">
       <c r="A64" s="3" t="n"/>
@@ -1676,6 +1788,7 @@
       <c r="E64" s="3" t="n"/>
       <c r="F64" s="3" t="n"/>
       <c r="G64" s="3" t="n"/>
+      <c r="H64" s="3" t="n"/>
     </row>
     <row r="65">
       <c r="A65" s="3" t="n"/>
@@ -1686,24 +1799,25 @@
       </c>
       <c r="C65" s="3" t="inlineStr">
         <is>
-          <t>דימה
-שבצוב</t>
+          <t>דובר
+כלפה</t>
         </is>
       </c>
       <c r="D65" s="3" t="inlineStr">
         <is>
-          <t>דותן
+          <t>משה
 שגיא</t>
         </is>
       </c>
       <c r="E65" s="3" t="inlineStr">
         <is>
-          <t>אסף
-אסרף</t>
+          <t>ארד
+יואל</t>
         </is>
       </c>
       <c r="F65" s="3" t="n"/>
       <c r="G65" s="3" t="n"/>
+      <c r="H65" s="3" t="n"/>
     </row>
     <row r="66">
       <c r="A66" s="3" t="n"/>
@@ -1717,6 +1831,7 @@
       <c r="E66" s="3" t="n"/>
       <c r="F66" s="3" t="n"/>
       <c r="G66" s="3" t="n"/>
+      <c r="H66" s="3" t="n"/>
     </row>
     <row r="67">
       <c r="A67" s="3" t="n"/>
@@ -1730,9 +1845,10 @@
       <c r="E67" s="3" t="n"/>
       <c r="F67" s="3" t="n"/>
       <c r="G67" s="3" t="n"/>
+      <c r="H67" s="3" t="n"/>
     </row>
   </sheetData>
-  <mergeCells count="77">
+  <mergeCells count="88">
     <mergeCell ref="A2:A23"/>
     <mergeCell ref="A24:A47"/>
     <mergeCell ref="A48:A67"/>
@@ -1810,6 +1926,17 @@
     <mergeCell ref="F46:F49"/>
     <mergeCell ref="F50:F53"/>
     <mergeCell ref="F54:F67"/>
+    <mergeCell ref="G2:G7"/>
+    <mergeCell ref="G8:G13"/>
+    <mergeCell ref="G14:G19"/>
+    <mergeCell ref="G20:G25"/>
+    <mergeCell ref="G26:G31"/>
+    <mergeCell ref="G32:G37"/>
+    <mergeCell ref="G38:G43"/>
+    <mergeCell ref="G44:G49"/>
+    <mergeCell ref="G50:G55"/>
+    <mergeCell ref="G56:G61"/>
+    <mergeCell ref="G62:G67"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Improve infinite loop and duos planning
</commit_message>
<xml_diff>
--- a/watch_list.xlsx
+++ b/watch_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andybenichou/Desktop/meshavsek/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A555C4E-A0E5-C44C-93BC-EB07F6CE6CE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C37A57B0-8104-FD49-B980-F43FCE659F36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="77">
   <si>
     <t>יום</t>
   </si>
@@ -43,25 +43,95 @@
     <t>כתת כוננות</t>
   </si>
   <si>
-    <t>שבת</t>
-  </si>
-  <si>
-    <t>08:00</t>
-  </si>
-  <si>
-    <t>שראל בלוך
-נתנאל שרעבי</t>
+    <t>20:00</t>
+  </si>
+  <si>
+    <t>אלכסיי ברומברג
+סרגיי לומיאנסקי</t>
   </si>
   <si>
     <t>דימטרי יוספוב
 סרגיי שבצוב</t>
   </si>
   <si>
-    <t>אור נצקנסקי
-עדן אסרף</t>
-  </si>
-  <si>
-    <t>6 תורני רס"פ - חדר</t>
+    <t>6 חדר</t>
+  </si>
+  <si>
+    <t>21:00</t>
+  </si>
+  <si>
+    <t>22:00</t>
+  </si>
+  <si>
+    <t>יהונתן דימנטמן
+ירין מטמוני</t>
+  </si>
+  <si>
+    <t>23:00</t>
+  </si>
+  <si>
+    <t>דעאל כהן
+אגומס מלדה</t>
+  </si>
+  <si>
+    <t>אנדי בנישו
+דוד סספורטס</t>
+  </si>
+  <si>
+    <t>ב</t>
+  </si>
+  <si>
+    <t>00:00</t>
+  </si>
+  <si>
+    <t>01:00</t>
+  </si>
+  <si>
+    <t>02:00</t>
+  </si>
+  <si>
+    <t>איתי סיני
+לוטם עטיה</t>
+  </si>
+  <si>
+    <t>איתי כהן
+עמיחי נעים</t>
+  </si>
+  <si>
+    <t>עדן אסרף
+אסף זבולון</t>
+  </si>
+  <si>
+    <t>7 חדר</t>
+  </si>
+  <si>
+    <t>03:00</t>
+  </si>
+  <si>
+    <t>04:00</t>
+  </si>
+  <si>
+    <t>05:00</t>
+  </si>
+  <si>
+    <t>אייל דבוש
+גיא פיאצה</t>
+  </si>
+  <si>
+    <t>06:00</t>
+  </si>
+  <si>
+    <t>8 תורני רס"פ - חדר</t>
+  </si>
+  <si>
+    <t>07:00</t>
+  </si>
+  <si>
+    <t>08:00</t>
+  </si>
+  <si>
+    <t>נדב קריספין
+יוסף רווה</t>
   </si>
   <si>
     <t>5 חדר</t>
@@ -76,18 +146,6 @@
     <t>11:00</t>
   </si>
   <si>
-    <t>אבנר איזרבביץ'
-סרגיי לומיאנסקי</t>
-  </si>
-  <si>
-    <t>איתי כהן
-נריה כלפה</t>
-  </si>
-  <si>
-    <t>לוטם עטיה
-איתי סיני</t>
-  </si>
-  <si>
     <t>12:00</t>
   </si>
   <si>
@@ -95,21 +153,13 @@
   </si>
   <si>
     <t>14:00</t>
-  </si>
-  <si>
-    <t>דעאל כהן
-שגיא אריה</t>
   </si>
   <si>
     <t>לואיס אברבוך
 אנזו גואטה</t>
   </si>
   <si>
-    <t>אנדי בנישו
-דוד סספורטס</t>
-  </si>
-  <si>
-    <t>11 חדר</t>
+    <t>10 חדר</t>
   </si>
   <si>
     <t>15:00</t>
@@ -121,16 +171,8 @@
     <t>17:00</t>
   </si>
   <si>
-    <t>מיכאל נפמן
-מאיר סדון</t>
-  </si>
-  <si>
-    <t>ארד רז
-יואל אודיז</t>
-  </si>
-  <si>
     <t>ליאור אבו חמדה
-משה אייכנשטין</t>
+שמעון ספנייב</t>
   </si>
   <si>
     <t>18:00</t>
@@ -139,151 +181,109 @@
     <t>19:00</t>
   </si>
   <si>
-    <t>20:00</t>
-  </si>
-  <si>
-    <t>נדב קריספין
-יוסף רווה</t>
-  </si>
-  <si>
-    <t>עדן אסרף
-אסף זבולון</t>
-  </si>
-  <si>
-    <t>דורון לביא
-שמעון ספנייב</t>
-  </si>
-  <si>
-    <t>10 חדר</t>
-  </si>
-  <si>
-    <t>21:00</t>
-  </si>
-  <si>
-    <t>22:00</t>
-  </si>
-  <si>
-    <t>מרדוש דהאן
-אור נצקנסקי</t>
-  </si>
-  <si>
-    <t>23:00</t>
-  </si>
-  <si>
-    <t>אייל דבוש
-גיא פיאצה</t>
-  </si>
-  <si>
-    <t>א</t>
-  </si>
-  <si>
-    <t>00:00</t>
-  </si>
-  <si>
-    <t>01:00</t>
-  </si>
-  <si>
-    <t>02:00</t>
+    <t>יונתן יונג
+נתנאל שרעבי</t>
   </si>
   <si>
     <t>דובר אלבז
 נריה כלפה</t>
   </si>
   <si>
-    <t>אלכסיי ברומברג
-סרגיי לומיאנסקי</t>
-  </si>
-  <si>
-    <t>יהונתן דימנטמן
-ירין מטמוני</t>
-  </si>
-  <si>
-    <t>אבנר איזרבביץ'
-עומרי דותן</t>
-  </si>
-  <si>
-    <t>9 חדר</t>
-  </si>
-  <si>
-    <t>03:00</t>
-  </si>
-  <si>
-    <t>04:00</t>
-  </si>
-  <si>
-    <t>05:00</t>
-  </si>
-  <si>
-    <t>איתי סיני
-לוטם עטיה</t>
-  </si>
-  <si>
-    <t>דעאל כהן
-אגומס מלדה</t>
-  </si>
-  <si>
-    <t>שגיא אריה
-איתי כהן</t>
-  </si>
-  <si>
-    <t>06:00</t>
-  </si>
-  <si>
-    <t>7 תורני רס"פ - חדר</t>
-  </si>
-  <si>
-    <t>07:00</t>
-  </si>
-  <si>
-    <t>8 חדר</t>
-  </si>
-  <si>
-    <t>ליאור אבו חמדה
-אנזו גואטה</t>
-  </si>
-  <si>
-    <t>לואיס אברבוך
-יונתן יונג</t>
-  </si>
-  <si>
-    <t>משה אייכנשטין
-שמעון ספנייב</t>
-  </si>
-  <si>
-    <t>מרדוש דהאן
-עמיחי נעים</t>
-  </si>
-  <si>
-    <t>עומרי דותן
-אור נצקנסקי</t>
-  </si>
-  <si>
-    <t>אבנר איזרבביץ'
-מיכאל ניסנוב</t>
-  </si>
-  <si>
-    <t>6 חדר</t>
-  </si>
-  <si>
-    <t>ב</t>
-  </si>
-  <si>
-    <t>איתי כהן
-עמיחי נעים</t>
-  </si>
-  <si>
-    <t>7 חדר</t>
-  </si>
-  <si>
-    <t>8 תורני רס"פ - חדר</t>
-  </si>
-  <si>
-    <t>עומרי דותן
-מיכאל ניסנוב</t>
+    <t>11 חדר</t>
   </si>
   <si>
     <t>יואל אודיז
 ארד רז</t>
+  </si>
+  <si>
+    <t>מרדוש דהן
+עומרי דותן</t>
+  </si>
+  <si>
+    <t>ג</t>
+  </si>
+  <si>
+    <t>לואיס אברבוך
+מיכאל ניסנוב</t>
+  </si>
+  <si>
+    <t>8 חדר</t>
+  </si>
+  <si>
+    <t>אנזו גואטה
+שמעון ספנייב</t>
+  </si>
+  <si>
+    <t>9 תורני רס"פ - חדר</t>
+  </si>
+  <si>
+    <t>משה אייכנשטין
+נתנאל שרעבי</t>
+  </si>
+  <si>
+    <t>ליאור אבו חמדה
+יונתן יונג</t>
+  </si>
+  <si>
+    <t>מרדוש דהן
+אסף זבולון</t>
+  </si>
+  <si>
+    <t>מיכאל נפמן
+מאור סדון</t>
+  </si>
+  <si>
+    <t>שגיא אריה
+דורון לביא</t>
+  </si>
+  <si>
+    <t>עומרי דותן
+איתי סיני</t>
+  </si>
+  <si>
+    <t>משה אייכנשטין
+מיכאל ניסנוב</t>
+  </si>
+  <si>
+    <t>ד</t>
+  </si>
+  <si>
+    <t>מרדוש דהן
+יונתן יונג</t>
+  </si>
+  <si>
+    <t>ליאור אבו חמדה
+אסף זבולון</t>
+  </si>
+  <si>
+    <t>9 חדר</t>
+  </si>
+  <si>
+    <t>עומרי דותן
+נתנאל שרעבי</t>
+  </si>
+  <si>
+    <t>10 תורני רס"פ - חדר</t>
+  </si>
+  <si>
+    <t>מיכאל ניסנוב
+איתי סיני</t>
+  </si>
+  <si>
+    <t>אבנר איזרבביץ
+דורון לביא</t>
+  </si>
+  <si>
+    <t>דעאל כהן
+שמעון ספנייב</t>
+  </si>
+  <si>
+    <t>אסף זבולון
+יונתן יונג</t>
+  </si>
+  <si>
+    <t>שגיא אריה
+שראל בלוך</t>
   </si>
 </sst>
 </file>
@@ -315,7 +315,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -338,11 +338,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -351,6 +360,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -655,10 +667,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H61"/>
+  <dimension ref="A1:H73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="F48" sqref="F48:F61"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -696,33 +708,33 @@
       <c r="H1" s="2"/>
     </row>
     <row r="2" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>7</v>
+      <c r="A2" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>12</v>
+        <v>41</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>30</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
       <c r="B3" s="2" t="s">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -734,7 +746,7 @@
     <row r="4" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="3"/>
       <c r="B4" s="2" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -746,16 +758,16 @@
     <row r="5" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="3"/>
       <c r="B5" s="2" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
@@ -764,7 +776,7 @@
     <row r="6" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="3"/>
       <c r="B6" s="2" t="s">
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -776,7 +788,7 @@
     <row r="7" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
       <c r="B7" s="2" t="s">
-        <v>21</v>
+        <v>48</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
@@ -788,27 +800,27 @@
     <row r="8" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="3"/>
       <c r="B8" s="2" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>23</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>24</v>
+        <v>49</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3" t="s">
-        <v>26</v>
+        <v>51</v>
       </c>
       <c r="H8" s="2"/>
     </row>
     <row r="9" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
       <c r="B9" s="2" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
@@ -820,37 +832,41 @@
     <row r="10" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="3"/>
       <c r="B10" s="2" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
+      <c r="F10" s="3" t="s">
+        <v>52</v>
+      </c>
       <c r="G10" s="3"/>
       <c r="H10" s="2"/>
     </row>
     <row r="11" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="3"/>
       <c r="B11" s="2" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>30</v>
+        <v>53</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
       <c r="H11" s="2"/>
     </row>
     <row r="12" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A12" s="3"/>
+      <c r="A12" s="3" t="s">
+        <v>54</v>
+      </c>
       <c r="B12" s="2" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
@@ -862,7 +878,7 @@
     <row r="13" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
       <c r="B13" s="2" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -874,27 +890,29 @@
     <row r="14" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="3"/>
       <c r="B14" s="2" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>36</v>
+        <v>55</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>37</v>
+        <v>8</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="F14" s="3"/>
+        <v>13</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="G14" s="3" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="H14" s="2"/>
     </row>
     <row r="15" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="3"/>
       <c r="B15" s="2" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
@@ -906,53 +924,51 @@
     <row r="16" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="3"/>
       <c r="B16" s="2" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
-      <c r="F16" s="3" t="s">
-        <v>42</v>
-      </c>
+      <c r="F16" s="3"/>
       <c r="G16" s="3"/>
       <c r="H16" s="2"/>
     </row>
     <row r="17" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="3"/>
       <c r="B17" s="2" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>10</v>
+        <v>57</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
       <c r="H17" s="2"/>
     </row>
     <row r="18" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
-        <v>45</v>
-      </c>
+      <c r="A18" s="3"/>
       <c r="B18" s="2" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
+      <c r="F18" s="3" t="s">
+        <v>58</v>
+      </c>
       <c r="G18" s="3"/>
       <c r="H18" s="2"/>
     </row>
     <row r="19" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="3"/>
       <c r="B19" s="2" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
@@ -964,29 +980,27 @@
     <row r="20" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="3"/>
       <c r="B20" s="2" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>50</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>52</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="F20" s="3"/>
       <c r="G20" s="3" t="s">
-        <v>53</v>
+        <v>10</v>
       </c>
       <c r="H20" s="2"/>
     </row>
     <row r="21" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="3"/>
       <c r="B21" s="2" t="s">
-        <v>54</v>
+        <v>35</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
@@ -998,7 +1012,7 @@
     <row r="22" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="3"/>
       <c r="B22" s="2" t="s">
-        <v>55</v>
+        <v>36</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
@@ -1010,16 +1024,16 @@
     <row r="23" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="3"/>
       <c r="B23" s="2" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
@@ -1028,21 +1042,19 @@
     <row r="24" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="3"/>
       <c r="B24" s="2" t="s">
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
-      <c r="F24" s="3" t="s">
-        <v>61</v>
-      </c>
+      <c r="F24" s="3"/>
       <c r="G24" s="3"/>
       <c r="H24" s="2"/>
     </row>
     <row r="25" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="3"/>
       <c r="B25" s="2" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
@@ -1054,27 +1066,27 @@
     <row r="26" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="3"/>
       <c r="B26" s="2" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>30</v>
+        <v>62</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>31</v>
+        <v>63</v>
       </c>
       <c r="F26" s="3"/>
       <c r="G26" s="3" t="s">
-        <v>63</v>
+        <v>24</v>
       </c>
       <c r="H26" s="2"/>
     </row>
     <row r="27" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="3"/>
       <c r="B27" s="2" t="s">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
@@ -1086,7 +1098,7 @@
     <row r="28" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="3"/>
       <c r="B28" s="2" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
@@ -1098,16 +1110,16 @@
     <row r="29" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="3"/>
       <c r="B29" s="2" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="C29" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E29" s="3" t="s">
         <v>64</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>65</v>
       </c>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
@@ -1116,7 +1128,7 @@
     <row r="30" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="3"/>
       <c r="B30" s="2" t="s">
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
@@ -1128,7 +1140,7 @@
     <row r="31" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="3"/>
       <c r="B31" s="2" t="s">
-        <v>21</v>
+        <v>48</v>
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
@@ -1140,25 +1152,27 @@
     <row r="32" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="3"/>
       <c r="B32" s="2" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>67</v>
+        <v>41</v>
       </c>
       <c r="F32" s="3"/>
-      <c r="G32" s="3"/>
+      <c r="G32" s="3" t="s">
+        <v>34</v>
+      </c>
       <c r="H32" s="2"/>
     </row>
     <row r="33" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="3"/>
       <c r="B33" s="2" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
@@ -1170,37 +1184,41 @@
     <row r="34" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="3"/>
       <c r="B34" s="2" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
-      <c r="F34" s="3"/>
+      <c r="F34" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="G34" s="3"/>
       <c r="H34" s="2"/>
     </row>
     <row r="35" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="3"/>
       <c r="B35" s="2" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>68</v>
+        <v>50</v>
       </c>
       <c r="F35" s="3"/>
       <c r="G35" s="3"/>
       <c r="H35" s="2"/>
     </row>
     <row r="36" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A36" s="3"/>
+      <c r="A36" s="3" t="s">
+        <v>66</v>
+      </c>
       <c r="B36" s="2" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
@@ -1212,7 +1230,7 @@
     <row r="37" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="3"/>
       <c r="B37" s="2" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
@@ -1224,27 +1242,29 @@
     <row r="38" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="3"/>
       <c r="B38" s="2" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>10</v>
+        <v>67</v>
       </c>
       <c r="E38" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G38" s="3" t="s">
         <v>69</v>
-      </c>
-      <c r="F38" s="3"/>
-      <c r="G38" s="3" t="s">
-        <v>70</v>
       </c>
       <c r="H38" s="2"/>
     </row>
     <row r="39" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="3"/>
       <c r="B39" s="2" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
@@ -1256,53 +1276,51 @@
     <row r="40" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="3"/>
       <c r="B40" s="2" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
-      <c r="F40" s="3" t="s">
-        <v>51</v>
-      </c>
+      <c r="F40" s="3"/>
       <c r="G40" s="3"/>
       <c r="H40" s="2"/>
     </row>
     <row r="41" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="3"/>
       <c r="B41" s="2" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>58</v>
+        <v>13</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>25</v>
+        <v>70</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>64</v>
+        <v>33</v>
       </c>
       <c r="F41" s="3"/>
       <c r="G41" s="3"/>
       <c r="H41" s="2"/>
     </row>
     <row r="42" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A42" s="3" t="s">
-        <v>71</v>
-      </c>
+      <c r="A42" s="3"/>
       <c r="B42" s="2" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
       <c r="E42" s="3"/>
-      <c r="F42" s="3"/>
+      <c r="F42" s="3" t="s">
+        <v>71</v>
+      </c>
       <c r="G42" s="3"/>
       <c r="H42" s="2"/>
     </row>
     <row r="43" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="3"/>
       <c r="B43" s="2" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
@@ -1314,29 +1332,27 @@
     <row r="44" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="3"/>
       <c r="B44" s="2" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>57</v>
+        <v>16</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="F44" s="3" t="s">
-        <v>37</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="F44" s="3"/>
       <c r="G44" s="3" t="s">
-        <v>73</v>
+        <v>51</v>
       </c>
       <c r="H44" s="2"/>
     </row>
     <row r="45" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="3"/>
       <c r="B45" s="2" t="s">
-        <v>54</v>
+        <v>35</v>
       </c>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
@@ -1348,7 +1364,7 @@
     <row r="46" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="3"/>
       <c r="B46" s="2" t="s">
-        <v>55</v>
+        <v>36</v>
       </c>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
@@ -1360,16 +1376,16 @@
     <row r="47" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="3"/>
       <c r="B47" s="2" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>66</v>
+        <v>41</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="F47" s="3"/>
       <c r="G47" s="3"/>
@@ -1378,21 +1394,19 @@
     <row r="48" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="3"/>
       <c r="B48" s="2" t="s">
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
       <c r="E48" s="3"/>
-      <c r="F48" s="3" t="s">
-        <v>74</v>
-      </c>
+      <c r="F48" s="3"/>
       <c r="G48" s="3"/>
       <c r="H48" s="2"/>
     </row>
     <row r="49" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="3"/>
       <c r="B49" s="2" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
@@ -1404,27 +1418,27 @@
     <row r="50" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="3"/>
       <c r="B50" s="2" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>10</v>
+        <v>62</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>44</v>
+        <v>73</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>9</v>
+        <v>74</v>
       </c>
       <c r="F50" s="3"/>
       <c r="G50" s="3" t="s">
-        <v>13</v>
+        <v>56</v>
       </c>
       <c r="H50" s="2"/>
     </row>
     <row r="51" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="3"/>
       <c r="B51" s="2" t="s">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
@@ -1436,7 +1450,7 @@
     <row r="52" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="3"/>
       <c r="B52" s="2" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="C52" s="3"/>
       <c r="D52" s="3"/>
@@ -1448,16 +1462,16 @@
     <row r="53" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="3"/>
       <c r="B53" s="2" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>51</v>
+        <v>75</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="F53" s="3"/>
       <c r="G53" s="3"/>
@@ -1466,7 +1480,7 @@
     <row r="54" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="3"/>
       <c r="B54" s="2" t="s">
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="C54" s="3"/>
       <c r="D54" s="3"/>
@@ -1478,7 +1492,7 @@
     <row r="55" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" s="3"/>
       <c r="B55" s="2" t="s">
-        <v>21</v>
+        <v>48</v>
       </c>
       <c r="C55" s="3"/>
       <c r="D55" s="3"/>
@@ -1487,138 +1501,109 @@
       <c r="G55" s="3"/>
       <c r="H55" s="2"/>
     </row>
-    <row r="56" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A56" s="3"/>
-      <c r="B56" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C56" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="D56" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E56" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F56" s="3"/>
-      <c r="G56" s="3" t="s">
-        <v>39</v>
-      </c>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="H56" s="2"/>
     </row>
-    <row r="57" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A57" s="3"/>
-      <c r="B57" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C57" s="3"/>
-      <c r="D57" s="3"/>
-      <c r="E57" s="3"/>
-      <c r="F57" s="3"/>
-      <c r="G57" s="3"/>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="H57" s="2"/>
     </row>
-    <row r="58" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A58" s="3"/>
-      <c r="B58" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C58" s="3"/>
-      <c r="D58" s="3"/>
-      <c r="E58" s="3"/>
-      <c r="F58" s="3"/>
-      <c r="G58" s="3"/>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="H58" s="2"/>
     </row>
-    <row r="59" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A59" s="3"/>
-      <c r="B59" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C59" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="D59" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E59" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="F59" s="3"/>
-      <c r="G59" s="3"/>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="H59" s="2"/>
     </row>
-    <row r="60" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A60" s="3"/>
-      <c r="B60" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C60" s="3"/>
-      <c r="D60" s="3"/>
-      <c r="E60" s="3"/>
-      <c r="F60" s="3"/>
-      <c r="G60" s="3"/>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="H60" s="2"/>
     </row>
-    <row r="61" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A61" s="3"/>
-      <c r="B61" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C61" s="3"/>
-      <c r="D61" s="3"/>
-      <c r="E61" s="3"/>
-      <c r="F61" s="3"/>
-      <c r="G61" s="3"/>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="H61" s="2"/>
     </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H62" s="2"/>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H63" s="2"/>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H64" s="2"/>
+    </row>
+    <row r="65" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H65" s="2"/>
+    </row>
+    <row r="66" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H66" s="2"/>
+    </row>
+    <row r="67" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H67" s="2"/>
+    </row>
+    <row r="68" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H68" s="2"/>
+    </row>
+    <row r="69" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H69" s="2"/>
+    </row>
+    <row r="70" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H70" s="2"/>
+    </row>
+    <row r="71" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H71" s="2"/>
+    </row>
+    <row r="72" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H72" s="2"/>
+    </row>
+    <row r="73" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H73" s="2"/>
+    </row>
   </sheetData>
-  <mergeCells count="79">
-    <mergeCell ref="F44:F47"/>
-    <mergeCell ref="F48:F61"/>
+  <mergeCells count="73">
+    <mergeCell ref="G44:G49"/>
+    <mergeCell ref="G50:G55"/>
+    <mergeCell ref="A2:A11"/>
+    <mergeCell ref="F2:F9"/>
+    <mergeCell ref="G14:G19"/>
+    <mergeCell ref="G20:G25"/>
+    <mergeCell ref="G26:G31"/>
+    <mergeCell ref="G32:G37"/>
+    <mergeCell ref="G38:G43"/>
     <mergeCell ref="G2:G7"/>
     <mergeCell ref="G8:G13"/>
-    <mergeCell ref="G14:G19"/>
-    <mergeCell ref="G20:G25"/>
-    <mergeCell ref="G26:G37"/>
-    <mergeCell ref="G38:G43"/>
-    <mergeCell ref="G44:G49"/>
-    <mergeCell ref="G50:G55"/>
-    <mergeCell ref="G56:G61"/>
-    <mergeCell ref="F2:F15"/>
-    <mergeCell ref="F16:F19"/>
-    <mergeCell ref="F20:F23"/>
-    <mergeCell ref="F24:F39"/>
-    <mergeCell ref="F40:F43"/>
+    <mergeCell ref="E44:E46"/>
     <mergeCell ref="E47:E49"/>
     <mergeCell ref="E50:E52"/>
     <mergeCell ref="E53:E55"/>
-    <mergeCell ref="E56:E58"/>
-    <mergeCell ref="E59:E61"/>
-    <mergeCell ref="D59:D61"/>
-    <mergeCell ref="E2:E4"/>
-    <mergeCell ref="E5:E7"/>
-    <mergeCell ref="E8:E10"/>
-    <mergeCell ref="E11:E13"/>
+    <mergeCell ref="F10:F13"/>
+    <mergeCell ref="F14:F17"/>
+    <mergeCell ref="F18:F33"/>
+    <mergeCell ref="F34:F37"/>
+    <mergeCell ref="F38:F41"/>
+    <mergeCell ref="F42:F55"/>
+    <mergeCell ref="E29:E31"/>
+    <mergeCell ref="E32:E34"/>
+    <mergeCell ref="E35:E37"/>
+    <mergeCell ref="E38:E40"/>
+    <mergeCell ref="E41:E43"/>
     <mergeCell ref="E14:E16"/>
     <mergeCell ref="E17:E19"/>
     <mergeCell ref="E20:E22"/>
     <mergeCell ref="E23:E25"/>
     <mergeCell ref="E26:E28"/>
-    <mergeCell ref="E29:E31"/>
-    <mergeCell ref="E32:E34"/>
-    <mergeCell ref="E35:E37"/>
-    <mergeCell ref="E38:E40"/>
-    <mergeCell ref="E41:E43"/>
-    <mergeCell ref="E44:E46"/>
+    <mergeCell ref="E2:E4"/>
+    <mergeCell ref="E5:E7"/>
+    <mergeCell ref="E8:E10"/>
+    <mergeCell ref="E11:E13"/>
+    <mergeCell ref="D41:D43"/>
     <mergeCell ref="D44:D46"/>
     <mergeCell ref="D47:D49"/>
     <mergeCell ref="D50:D52"/>
     <mergeCell ref="D53:D55"/>
-    <mergeCell ref="D56:D58"/>
-    <mergeCell ref="C56:C58"/>
-    <mergeCell ref="C59:C61"/>
+    <mergeCell ref="D26:D28"/>
+    <mergeCell ref="D29:D31"/>
+    <mergeCell ref="D32:D34"/>
+    <mergeCell ref="D35:D37"/>
+    <mergeCell ref="D38:D40"/>
+    <mergeCell ref="C50:C52"/>
+    <mergeCell ref="C53:C55"/>
     <mergeCell ref="D2:D4"/>
     <mergeCell ref="D5:D7"/>
     <mergeCell ref="D8:D10"/>
@@ -1627,34 +1612,26 @@
     <mergeCell ref="D17:D19"/>
     <mergeCell ref="D20:D22"/>
     <mergeCell ref="D23:D25"/>
-    <mergeCell ref="D26:D28"/>
-    <mergeCell ref="D29:D31"/>
-    <mergeCell ref="D32:D34"/>
-    <mergeCell ref="D35:D37"/>
-    <mergeCell ref="D38:D40"/>
-    <mergeCell ref="D41:D43"/>
+    <mergeCell ref="C35:C37"/>
+    <mergeCell ref="C38:C40"/>
     <mergeCell ref="C41:C43"/>
     <mergeCell ref="C44:C46"/>
     <mergeCell ref="C47:C49"/>
-    <mergeCell ref="C50:C52"/>
-    <mergeCell ref="C53:C55"/>
-    <mergeCell ref="A2:A17"/>
-    <mergeCell ref="A18:A41"/>
-    <mergeCell ref="A42:A61"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="C23:C25"/>
+    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="C29:C31"/>
+    <mergeCell ref="C32:C34"/>
+    <mergeCell ref="A12:A35"/>
+    <mergeCell ref="A36:A55"/>
     <mergeCell ref="C2:C4"/>
     <mergeCell ref="C5:C7"/>
     <mergeCell ref="C8:C10"/>
     <mergeCell ref="C11:C13"/>
     <mergeCell ref="C14:C16"/>
     <mergeCell ref="C17:C19"/>
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="C23:C25"/>
-    <mergeCell ref="C26:C28"/>
-    <mergeCell ref="C29:C31"/>
-    <mergeCell ref="C32:C34"/>
-    <mergeCell ref="C35:C37"/>
-    <mergeCell ref="C38:C40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add custom time range missing in excel
</commit_message>
<xml_diff>
--- a/watch_list.xlsx
+++ b/watch_list.xlsx
@@ -506,7 +506,7 @@
   <cols>
     <col width="21" customWidth="1" min="1" max="1"/>
     <col width="7" customWidth="1" min="2" max="2"/>
-    <col width="29" customWidth="1" min="3" max="3"/>
+    <col width="28" customWidth="1" min="3" max="3"/>
     <col width="28" customWidth="1" min="4" max="4"/>
     <col width="27" customWidth="1" min="5" max="5"/>
     <col width="8" customWidth="1" min="6" max="6"/>
@@ -1968,7 +1968,7 @@
       <c r="E88" s="3" t="inlineStr">
         <is>
           <t>עומרי דותן
-אבנר יוזפוביץ</t>
+דעאל כהן</t>
         </is>
       </c>
       <c r="F88" s="6" t="n"/>
@@ -1988,7 +1988,7 @@
       </c>
       <c r="D89" s="3" t="inlineStr">
         <is>
-          <t>מרדוש דהן
+          <t>אבנר יוזפוביץ
 יניב משה</t>
         </is>
       </c>
@@ -2030,20 +2030,20 @@
       </c>
       <c r="C92" s="3" t="inlineStr">
         <is>
+          <t>עדן אסרף
+איתי סיני</t>
+        </is>
+      </c>
+      <c r="D92" s="3" t="inlineStr">
+        <is>
           <t>ליאור אבו חמדה
-מיכאל ניסנוב</t>
-        </is>
-      </c>
-      <c r="D92" s="3" t="inlineStr">
+מרדוש דהן</t>
+        </is>
+      </c>
+      <c r="E92" s="3" t="inlineStr">
         <is>
           <t>שראל בלוך
 נתנאל שרעבי</t>
-        </is>
-      </c>
-      <c r="E92" s="3" t="inlineStr">
-        <is>
-          <t>עדן אסרף
-איתי סיני</t>
         </is>
       </c>
       <c r="F92" s="6" t="n"/>
@@ -2138,7 +2138,7 @@
       <c r="D98" s="3" t="inlineStr">
         <is>
           <t>אסף זבולון
-דורון לביא</t>
+אדיר מור</t>
         </is>
       </c>
       <c r="E98" s="6" t="n"/>
@@ -2181,13 +2181,13 @@
       </c>
       <c r="C101" s="3" t="inlineStr">
         <is>
-          <t>לואיס אברבוך
-זיטר יצחק</t>
+          <t>איתמר בנימין
+מיכאל ניסנוב</t>
         </is>
       </c>
       <c r="D101" s="3" t="inlineStr">
         <is>
-          <t>אדיר מור
+          <t>דורון לביא
 עמיחי נעים</t>
         </is>
       </c>
@@ -2319,8 +2319,8 @@
       </c>
       <c r="C110" s="3" t="inlineStr">
         <is>
-          <t>איתמר בנימין
-פביאן חויוס</t>
+          <t>לואיס אברבוך
+זיטר יצחק</t>
         </is>
       </c>
       <c r="D110" s="3" t="inlineStr">
@@ -2486,7 +2486,7 @@
   <cols>
     <col width="21" customWidth="1" min="1" max="1"/>
     <col width="7" customWidth="1" min="2" max="2"/>
-    <col width="270" customWidth="1" min="3" max="3"/>
+    <col width="269" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3008,8 +3008,8 @@
       <c r="C44" s="3" t="inlineStr">
         <is>
           <t>שגיא אריה, דעאל כהן, עדן אסרף, איתי סיני, דובר אלבז
-נריה כלפה, זיטר יצחק, נדב קריספין, יוסף רווה, פביאן חויוס
-ראובן מאור, ארד רז</t>
+נריה כלפה, זיטר יצחק, נדב קריספין, יוסף רווה, ראובן מאור
+ארד רז</t>
         </is>
       </c>
     </row>
@@ -3041,8 +3041,7 @@
       <c r="C47" s="3" t="inlineStr">
         <is>
           <t>דעאל כהן, אבנר יוזפוביץ, עדן אסרף, איתי סיני, דובר אלבז
-נריה כלפה, חן טלה, פביאן חויוס, ראובן מאור, יואל אודיז
-ארד רז</t>
+נריה כלפה, חן טלה, ראובן מאור, יואל אודיז, ארד רז</t>
         </is>
       </c>
     </row>
@@ -3056,8 +3055,8 @@
       <c r="C48" s="3" t="inlineStr">
         <is>
           <t>דעאל כהן, אבנר יוזפוביץ, יניב משה, עדן אסרף, איתי סיני
-דובר אלבז, נריה כלפה, חן טלה, אור נצקנסקי, פביאן חויוס
-ראובן מאור, יואל אודיז, ארד רז</t>
+דובר אלבז, נריה כלפה, חן טלה, אור נצקנסקי, ראובן מאור
+יואל אודיז, ארד רז</t>
         </is>
       </c>
     </row>
@@ -3384,7 +3383,7 @@
       </c>
       <c r="C76" s="3" t="inlineStr">
         <is>
-          <t>דעאל כהן, אגומס מלדה, ליאור אבו חמדה, יניב משה, עדן אסרף
+          <t>אגומס מלדה, אבנר יוזפוביץ, ליאור אבו חמדה, יניב משה, עדן אסרף
 איתי סיני, מרדוש דהן, שראל בלוך, נתנאל שרעבי, אייל דבוש
 גיא פיאצה</t>
         </is>
@@ -3399,8 +3398,9 @@
       </c>
       <c r="C77" s="3" t="inlineStr">
         <is>
-          <t>ליאור אבו חמדה, עדן אסרף, איתי סיני, שראל בלוך, נתנאל שרעבי
-אייל דבוש, גיא פיאצה, דובר אלבז, נריה כלפה, חן טלה</t>
+          <t>ליאור אבו חמדה, עדן אסרף, איתי סיני, מרדוש דהן, שראל בלוך
+נתנאל שרעבי, אייל דבוש, גיא פיאצה, דובר אלבז, נריה כלפה
+חן טלה</t>
         </is>
       </c>
     </row>
@@ -3432,7 +3432,7 @@
       <c r="C80" s="3" t="inlineStr">
         <is>
           <t>אייל דבוש, גיא פיאצה, דובר אלבז, נריה כלפה, חן טלה
-אסף זבולון, אדיר מור, לוטם עטיה</t>
+אסף זבולון, אדיר מור, מיכאל ניסנוב, לוטם עטיה</t>
         </is>
       </c>
     </row>
@@ -3463,8 +3463,8 @@
       </c>
       <c r="C83" s="3" t="inlineStr">
         <is>
-          <t>חן טלה, אסף זבולון, אדיר מור, לוטם עטיה, דורון לביא
-עמיחי נעים, איתמר בנימין, זיטר יצחק</t>
+          <t>חן טלה, אסף זבולון, אדיר מור, מיכאל ניסנוב, לוטם עטיה
+דורון לביא, עמיחי נעים, איתמר בנימין, זיטר יצחק</t>
         </is>
       </c>
     </row>
@@ -3497,8 +3497,8 @@
       </c>
       <c r="C86" s="3" t="inlineStr">
         <is>
-          <t>אדיר מור, עמיחי נעים, איתמר בנימין, זיטר יצחק, נדב קריספין
-יוסף רווה, לואיס אברבוך, פביאן חויוס</t>
+          <t>מיכאל ניסנוב, דורון לביא, עמיחי נעים, איתמר בנימין, זיטר יצחק
+נדב קריספין, יוסף רווה, לואיס אברבוך, פביאן חויוס</t>
         </is>
       </c>
     </row>
@@ -3529,8 +3529,8 @@
       </c>
       <c r="C89" s="3" t="inlineStr">
         <is>
-          <t>איתמר בנימין, נדב קריספין, יוסף רווה, פביאן חויוס, אלכסיי ברומברג
-ראובן מאור, יואל אודיז, ארד רז</t>
+          <t>זיטר יצחק, נדב קריספין, יוסף רווה, לואיס אברבוך, פביאן חויוס
+אלכסיי ברומברג, ראובן מאור, יואל אודיז, ארד רז</t>
         </is>
       </c>
     </row>
@@ -3562,7 +3562,7 @@
       <c r="C92" s="3" t="inlineStr">
         <is>
           <t>דעאל כהן, אגומס מלדה, עומרי דותן, אבנר יוזפוביץ, יניב משה
-מרדוש דהן, איתמר בנימין, נדב קריספין, יוסף רווה, פביאן חויוס
+זיטר יצחק, נדב קריספין, יוסף רווה, לואיס אברבוך, פביאן חויוס
 אלכסיי ברומברג, ראובן מאור, יואל אודיז, ארד רז</t>
         </is>
       </c>
@@ -3595,8 +3595,8 @@
       <c r="C95" s="3" t="inlineStr">
         <is>
           <t>דעאל כהן, אגומס מלדה, עומרי דותן, אבנר יוזפוביץ, ליאור אבו חמדה
-יניב משה, מרדוש דהן, שראל בלוך, נתנאל שרעבי, מיכאל ניסנוב
-איתמר בנימין, נדב קריספין, יוסף רווה, פביאן חויוס, אלכסיי ברומברג
+יניב משה, עדן אסרף, איתי סיני, מרדוש דהן, זיטר יצחק
+נדב קריספין, יוסף רווה, לואיס אברבוך, פביאן חויוס, אלכסיי ברומברג
 ראובן מאור, יואל אודיז, ארד רז</t>
         </is>
       </c>
@@ -3612,8 +3612,8 @@
         <is>
           <t>שגיא אריה, דעאל כהן, אגומס מלדה, עומרי דותן, אבנר יוזפוביץ
 ליאור אבו חמדה, יניב משה, עדן אסרף, איתי סיני, מרדוש דהן
-שראל בלוך, נתנאל שרעבי, אור נצקנסקי, מיכאל ניסנוב, איתמר בנימין
-נדב קריספין, יוסף רווה, פביאן חויוס, אלכסיי ברומברג, ראובן מאור
+שראל בלוך, נתנאל שרעבי, אור נצקנסקי, זיטר יצחק, נדב קריספין
+יוסף רווה, לואיס אברבוך, פביאן חויוס, אלכסיי ברומברג, ראובן מאור
 יואל אודיז, ארד רז</t>
         </is>
       </c>
@@ -3639,7 +3639,7 @@
           <t>דעאל כהן, אגומס מלדה, עומרי דותן, אבנר יוזפוביץ, ליאור אבו חמדה
 יניב משה, עדן אסרף, איתי סיני, מרדוש דהן, שראל בלוך
 נתנאל שרעבי, אייל דבוש, גיא פיאצה, דובר אלבז, נריה כלפה
-אור נצקנסקי, מיכאל ניסנוב, נדב קריספין, יוסף רווה, אלכסיי ברומברג
+אור נצקנסקי, נדב קריספין, יוסף רווה, פביאן חויוס, אלכסיי ברומברג
 ראובן מאור, יואל אודיז, ארד רז</t>
         </is>
       </c>

</xml_diff>